<commit_message>
Improved peak detection and percentage data retained
</commit_message>
<xml_diff>
--- a/fly_record.xlsx
+++ b/fly_record.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\group_swinderen\Dinis\Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\group_swinderen\Dinis\Sequential Effects ERP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04610227-5482-45B4-B7F1-B16893695527}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C616732-E978-43DC-A235-948E03DED788}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{0C11348E-E482-4597-B3FE-1374AFB87193}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Bruno: A bit iffy; Dinis: it's fine</t>
+  </si>
+  <si>
+    <t>Crashed around 50 mins</t>
   </si>
 </sst>
 </file>
@@ -460,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680E0717-9BF1-4D4C-A430-96F9A20E59A5}">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="I108" sqref="I108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2352,6 +2355,1343 @@
         <v>14</v>
       </c>
     </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B68">
+        <v>19</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E68">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F68">
+        <f>5*1/200</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G68">
+        <f>1/(E68+F68)</f>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B69" s="4">
+        <v>19</v>
+      </c>
+      <c r="C69">
+        <v>8</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" s="4">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F69" s="4">
+        <f>5*1/200</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G69" s="4">
+        <f t="shared" ref="G69:G113" si="10">1/(E69+F69)</f>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="H69" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B70" s="4">
+        <v>19</v>
+      </c>
+      <c r="C70">
+        <v>6</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F70">
+        <f>7*1/200</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G70" s="4">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="H70" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B71" s="4">
+        <v>19</v>
+      </c>
+      <c r="C71">
+        <v>7</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" s="4">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F71" s="4">
+        <f>7*1/200</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G71" s="4">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="H71" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B72" s="4">
+        <v>19</v>
+      </c>
+      <c r="C72">
+        <v>9</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E72">
+        <f>2*1/200</f>
+        <v>0.01</v>
+      </c>
+      <c r="F72">
+        <f>14*1/200</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G72" s="4">
+        <f t="shared" si="10"/>
+        <v>12.5</v>
+      </c>
+      <c r="H72" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B73" s="4">
+        <v>19</v>
+      </c>
+      <c r="C73">
+        <v>10</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="4">
+        <f>2*1/200</f>
+        <v>0.01</v>
+      </c>
+      <c r="F73" s="4">
+        <f>14*1/200</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G73" s="4">
+        <f t="shared" si="10"/>
+        <v>12.5</v>
+      </c>
+      <c r="H73" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B74" s="4">
+        <v>19</v>
+      </c>
+      <c r="C74">
+        <v>11</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E74">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="F74">
+        <f>28*1/200</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G74" s="4">
+        <f t="shared" si="10"/>
+        <v>6.25</v>
+      </c>
+      <c r="H74" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B75" s="4">
+        <v>19</v>
+      </c>
+      <c r="C75">
+        <v>12</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" s="4">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="F75" s="4">
+        <f>28*1/200</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G75" s="4">
+        <f t="shared" si="10"/>
+        <v>6.25</v>
+      </c>
+      <c r="H75" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B76" s="4">
+        <v>19</v>
+      </c>
+      <c r="C76">
+        <v>13</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76">
+        <f>20*1/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="F76">
+        <f>140*1/200</f>
+        <v>0.7</v>
+      </c>
+      <c r="G76" s="4">
+        <f t="shared" si="10"/>
+        <v>1.25</v>
+      </c>
+      <c r="H76" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B77" s="4">
+        <v>19</v>
+      </c>
+      <c r="C77">
+        <v>14</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" s="4">
+        <f>20*1/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="F77" s="4">
+        <f>140*1/200</f>
+        <v>0.7</v>
+      </c>
+      <c r="G77" s="4">
+        <f t="shared" si="10"/>
+        <v>1.25</v>
+      </c>
+      <c r="H77" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B78" s="4">
+        <v>19</v>
+      </c>
+      <c r="C78">
+        <v>15</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E78">
+        <f>1*1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F78">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="G78" s="4">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="H78" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B79" s="4">
+        <v>19</v>
+      </c>
+      <c r="C79">
+        <v>16</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" s="4">
+        <f>1*1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F79" s="4">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="G79" s="4">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="H79" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B80">
+        <v>20</v>
+      </c>
+      <c r="C80">
+        <v>8</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E80" s="4">
+        <f>2*1/200</f>
+        <v>0.01</v>
+      </c>
+      <c r="F80" s="4">
+        <f>14*1/200</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G80" s="4">
+        <f t="shared" si="10"/>
+        <v>12.5</v>
+      </c>
+      <c r="H80" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B81" s="4">
+        <v>20</v>
+      </c>
+      <c r="C81">
+        <v>9</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81" s="4">
+        <f>2*1/200</f>
+        <v>0.01</v>
+      </c>
+      <c r="F81" s="4">
+        <f>14*1/200</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G81" s="4">
+        <f t="shared" si="10"/>
+        <v>12.5</v>
+      </c>
+      <c r="H81" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B82" s="4">
+        <v>20</v>
+      </c>
+      <c r="C82">
+        <v>10</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E82" s="4">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="F82" s="4">
+        <f>28*1/200</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G82" s="4">
+        <f t="shared" si="10"/>
+        <v>6.25</v>
+      </c>
+      <c r="H82" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B83" s="4">
+        <v>20</v>
+      </c>
+      <c r="C83">
+        <v>11</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E83" s="4">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="F83" s="4">
+        <f>28*1/200</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G83" s="4">
+        <f t="shared" si="10"/>
+        <v>6.25</v>
+      </c>
+      <c r="H83" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B84" s="4">
+        <v>20</v>
+      </c>
+      <c r="C84">
+        <v>12</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E84" s="4">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F84" s="4">
+        <f>7*1/200</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G84" s="4">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="H84" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B85" s="4">
+        <v>20</v>
+      </c>
+      <c r="C85">
+        <v>13</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" s="4">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F85" s="4">
+        <f>7*1/200</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G85" s="4">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="H85" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B86" s="4">
+        <v>20</v>
+      </c>
+      <c r="C86">
+        <v>14</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E86" s="4">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F86" s="4">
+        <f>5*1/200</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G86" s="4">
+        <f t="shared" si="10"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="H86" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B87" s="4">
+        <v>20</v>
+      </c>
+      <c r="C87">
+        <v>15</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" s="4">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F87" s="4">
+        <f>5*1/200</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G87" s="4">
+        <f t="shared" si="10"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="H87" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B88" s="4">
+        <v>20</v>
+      </c>
+      <c r="C88">
+        <v>16</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E88" s="4">
+        <f>1*1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F88" s="4">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="G88" s="4">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="H88" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B89" s="4">
+        <v>20</v>
+      </c>
+      <c r="C89">
+        <v>17</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E89" s="4">
+        <f>1*1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F89" s="4">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="G89" s="4">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="H89" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B90" s="4">
+        <v>20</v>
+      </c>
+      <c r="C90">
+        <v>23</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E90" s="4">
+        <f>20*1/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="F90" s="4">
+        <f>140*1/200</f>
+        <v>0.7</v>
+      </c>
+      <c r="G90" s="4">
+        <f t="shared" si="10"/>
+        <v>1.25</v>
+      </c>
+      <c r="H90" s="4">
+        <v>0</v>
+      </c>
+      <c r="I90" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B91" s="4">
+        <v>20</v>
+      </c>
+      <c r="C91">
+        <v>24</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" s="4">
+        <f>20*1/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="F91" s="4">
+        <f>140*1/200</f>
+        <v>0.7</v>
+      </c>
+      <c r="G91" s="4">
+        <f t="shared" si="10"/>
+        <v>1.25</v>
+      </c>
+      <c r="H91" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B92">
+        <v>21</v>
+      </c>
+      <c r="C92">
+        <v>29</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E92" s="4">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="F92" s="4">
+        <f>28*1/200</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G92" s="4">
+        <f t="shared" si="10"/>
+        <v>6.25</v>
+      </c>
+      <c r="H92" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B93" s="4">
+        <v>21</v>
+      </c>
+      <c r="C93">
+        <v>30</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" s="4">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="F93" s="4">
+        <f>28*1/200</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G93" s="4">
+        <f t="shared" si="10"/>
+        <v>6.25</v>
+      </c>
+      <c r="H93" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B94" s="4">
+        <v>21</v>
+      </c>
+      <c r="C94">
+        <v>31</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E94" s="4">
+        <f>2*1/200</f>
+        <v>0.01</v>
+      </c>
+      <c r="F94" s="4">
+        <f>14*1/200</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G94" s="4">
+        <f t="shared" si="10"/>
+        <v>12.5</v>
+      </c>
+      <c r="H94" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B95" s="4">
+        <v>21</v>
+      </c>
+      <c r="C95">
+        <v>32</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E95" s="4">
+        <f>2*1/200</f>
+        <v>0.01</v>
+      </c>
+      <c r="F95" s="4">
+        <f>14*1/200</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G95" s="4">
+        <f t="shared" si="10"/>
+        <v>12.5</v>
+      </c>
+      <c r="H95" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B96" s="4">
+        <v>21</v>
+      </c>
+      <c r="C96">
+        <v>33</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E96" s="4">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F96" s="4">
+        <f>7*1/200</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G96" s="4">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="H96" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B97" s="4">
+        <v>21</v>
+      </c>
+      <c r="C97">
+        <v>34</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E97" s="4">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F97" s="4">
+        <f>7*1/200</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G97" s="4">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="H97" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B98" s="4">
+        <v>21</v>
+      </c>
+      <c r="C98">
+        <v>35</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E98" s="4">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F98" s="4">
+        <f>5*1/200</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G98" s="4">
+        <f t="shared" si="10"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="H98" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B99" s="4">
+        <v>21</v>
+      </c>
+      <c r="C99">
+        <v>36</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E99" s="4">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F99" s="4">
+        <f>5*1/200</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G99" s="4">
+        <f t="shared" si="10"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="H99" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B100" s="4">
+        <v>21</v>
+      </c>
+      <c r="C100">
+        <v>37</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E100" s="4">
+        <f>1*1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F100" s="4">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="G100" s="4">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="H100" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B101" s="4">
+        <v>21</v>
+      </c>
+      <c r="C101">
+        <v>38</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E101" s="4">
+        <f>1*1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F101" s="4">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="G101" s="4">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="H101" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>44547</v>
+      </c>
+      <c r="B102" s="4">
+        <v>22</v>
+      </c>
+      <c r="C102">
+        <v>7</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E102" s="4">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="F102" s="4">
+        <f>28*1/200</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G102" s="4">
+        <f t="shared" si="10"/>
+        <v>6.25</v>
+      </c>
+      <c r="H102" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>44547</v>
+      </c>
+      <c r="B103" s="4">
+        <v>22</v>
+      </c>
+      <c r="C103">
+        <v>8</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E103" s="4">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="F103" s="4">
+        <f>28*1/200</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G103" s="4">
+        <f t="shared" si="10"/>
+        <v>6.25</v>
+      </c>
+      <c r="H103" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>44547</v>
+      </c>
+      <c r="B104" s="4">
+        <v>22</v>
+      </c>
+      <c r="C104">
+        <v>9</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E104" s="4">
+        <f>2*1/200</f>
+        <v>0.01</v>
+      </c>
+      <c r="F104" s="4">
+        <f>14*1/200</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G104" s="4">
+        <f t="shared" si="10"/>
+        <v>12.5</v>
+      </c>
+      <c r="H104" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>44547</v>
+      </c>
+      <c r="B105" s="4">
+        <v>22</v>
+      </c>
+      <c r="C105">
+        <v>10</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E105" s="4">
+        <f>2*1/200</f>
+        <v>0.01</v>
+      </c>
+      <c r="F105" s="4">
+        <f>14*1/200</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G105" s="4">
+        <f t="shared" si="10"/>
+        <v>12.5</v>
+      </c>
+      <c r="H105" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>44547</v>
+      </c>
+      <c r="B106" s="4">
+        <v>22</v>
+      </c>
+      <c r="C106">
+        <v>11</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E106" s="4">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F106" s="4">
+        <f>7*1/200</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G106" s="4">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="H106" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>44547</v>
+      </c>
+      <c r="B107" s="4">
+        <v>22</v>
+      </c>
+      <c r="C107">
+        <v>12</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E107" s="4">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F107" s="4">
+        <f>7*1/200</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G107" s="4">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="H107" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>44547</v>
+      </c>
+      <c r="B108" s="4">
+        <v>22</v>
+      </c>
+      <c r="C108">
+        <v>13</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E108" s="4">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F108" s="4">
+        <f>5*1/200</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G108" s="4">
+        <f t="shared" si="10"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="H108" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>44547</v>
+      </c>
+      <c r="B109" s="4">
+        <v>22</v>
+      </c>
+      <c r="C109">
+        <v>14</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" s="4">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F109" s="4">
+        <f>5*1/200</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G109" s="4">
+        <f t="shared" si="10"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="H109" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>44547</v>
+      </c>
+      <c r="B110" s="4">
+        <v>22</v>
+      </c>
+      <c r="C110">
+        <v>15</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E110" s="4">
+        <f>1*1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F110" s="4">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="G110" s="4">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="H110" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>44547</v>
+      </c>
+      <c r="B111" s="4">
+        <v>22</v>
+      </c>
+      <c r="C111">
+        <v>16</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E111" s="4">
+        <f>1*1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F111" s="4">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="G111" s="4">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="H111" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>44547</v>
+      </c>
+      <c r="B112" s="4">
+        <v>22</v>
+      </c>
+      <c r="C112">
+        <v>17</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E112" s="4">
+        <f>20*1/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="F112" s="4">
+        <f>140*1/200</f>
+        <v>0.7</v>
+      </c>
+      <c r="G112" s="4">
+        <f t="shared" si="10"/>
+        <v>1.25</v>
+      </c>
+      <c r="H112" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>44547</v>
+      </c>
+      <c r="B113" s="4">
+        <v>22</v>
+      </c>
+      <c r="C113">
+        <v>18</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E113" s="4">
+        <f>20*1/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="F113" s="4">
+        <f>140*1/200</f>
+        <v>0.7</v>
+      </c>
+      <c r="G113" s="4">
+        <f t="shared" si="10"/>
+        <v>1.25</v>
+      </c>
+      <c r="H113" s="4">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Addded preprocess script and minor changes
</commit_message>
<xml_diff>
--- a/fly_record.xlsx
+++ b/fly_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\group_swinderen\Dinis\Sequential Effects ERP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0AF463-4177-411F-AAFA-5B33E2D903C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112C1A25-3DB2-4369-B794-F7C22BA1A51A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{0C11348E-E482-4597-B3FE-1374AFB87193}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -102,7 +102,10 @@
     <t>Glued legs not cut</t>
   </si>
   <si>
-    <t>Glued legs not cut; Jitter due to clicking anotehr window</t>
+    <t>Data a bit iffy</t>
+  </si>
+  <si>
+    <t>Glued legs not cut; Jitter due to clicking another window</t>
   </si>
 </sst>
 </file>
@@ -471,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680E0717-9BF1-4D4C-A430-96F9A20E59A5}">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="I113" sqref="I113"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="I108" sqref="I108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,6 +1072,9 @@
       <c r="H22" s="4">
         <v>0</v>
       </c>
+      <c r="I22" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -2383,8 +2389,8 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G68">
-        <f>1/(E68+F68)</f>
-        <v>33.333333333333329</v>
+        <f>33.3</f>
+        <v>33.299999999999997</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -2412,8 +2418,8 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G69" s="4">
-        <f t="shared" ref="G69:G113" si="10">1/(E69+F69)</f>
-        <v>33.333333333333329</v>
+        <f>33.3</f>
+        <v>33.299999999999997</v>
       </c>
       <c r="H69" s="4">
         <v>0</v>
@@ -2441,7 +2447,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="G70" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="G69:G113" si="10">1/(E70+F70)</f>
         <v>25</v>
       </c>
       <c r="H70" s="4">
@@ -2905,8 +2911,8 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G86" s="4">
-        <f t="shared" si="10"/>
-        <v>33.333333333333329</v>
+        <f t="shared" ref="G86:G87" si="11">33.3</f>
+        <v>33.299999999999997</v>
       </c>
       <c r="H86" s="4">
         <v>0</v>
@@ -2934,8 +2940,8 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G87" s="4">
-        <f t="shared" si="10"/>
-        <v>33.333333333333329</v>
+        <f t="shared" si="11"/>
+        <v>33.299999999999997</v>
       </c>
       <c r="H87" s="4">
         <v>0</v>
@@ -3256,8 +3262,8 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G98" s="4">
-        <f t="shared" si="10"/>
-        <v>33.333333333333329</v>
+        <f t="shared" ref="G98:G99" si="12">33.3</f>
+        <v>33.299999999999997</v>
       </c>
       <c r="H98" s="4">
         <v>0</v>
@@ -3285,8 +3291,8 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G99" s="4">
-        <f t="shared" si="10"/>
-        <v>33.333333333333329</v>
+        <f t="shared" si="12"/>
+        <v>33.299999999999997</v>
       </c>
       <c r="H99" s="4">
         <v>0</v>
@@ -3564,8 +3570,8 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G108" s="4">
-        <f t="shared" si="10"/>
-        <v>33.333333333333329</v>
+        <f t="shared" ref="G108:G109" si="13">33.3</f>
+        <v>33.299999999999997</v>
       </c>
       <c r="H108" s="4">
         <v>0</v>
@@ -3596,8 +3602,8 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G109" s="4">
-        <f t="shared" si="10"/>
-        <v>33.333333333333329</v>
+        <f t="shared" si="13"/>
+        <v>33.299999999999997</v>
       </c>
       <c r="H109" s="4">
         <v>0</v>
@@ -3731,7 +3737,7 @@
         <v>0</v>
       </c>
       <c r="I113" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed end trimming jitter
</commit_message>
<xml_diff>
--- a/fly_record.xlsx
+++ b/fly_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\group_swinderen\Dinis\Sequential Effects ERP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D28B2F-586E-40BE-B50E-6AB2F01AAEA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAFAA29-0820-4B6B-8E61-B97E0DEFE056}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10800" windowHeight="5190" xr2:uid="{0C11348E-E482-4597-B3FE-1374AFB87193}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>regular</t>
+  </si>
+  <si>
+    <t>alternating to calibrate</t>
   </si>
 </sst>
 </file>
@@ -554,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680E0717-9BF1-4D4C-A430-96F9A20E59A5}">
-  <dimension ref="A1:I195"/>
+  <dimension ref="A1:I200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
-      <selection activeCell="H197" sqref="H197"/>
+      <selection activeCell="F197" sqref="F197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6023,93 +6026,95 @@
       <c r="H187" s="5">
         <v>0</v>
       </c>
-      <c r="I187" s="5"/>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="6">
         <v>44595</v>
       </c>
-      <c r="B188" s="5">
+      <c r="B188">
         <v>29</v>
       </c>
-      <c r="C188" s="5">
-        <v>4</v>
+      <c r="C188">
+        <v>1</v>
       </c>
       <c r="D188" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E188" s="5">
+        <f>1*1/200</f>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F188" s="5">
-        <v>3.5000000000000003E-2</v>
+        <f>4*1/200</f>
+        <v>0.02</v>
       </c>
       <c r="G188" s="5">
-        <v>25</v>
+        <f t="shared" ref="G188" si="18">1/(E188+F188)</f>
+        <v>40</v>
       </c>
       <c r="H188" s="5">
         <v>0</v>
       </c>
       <c r="I188" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="6">
         <v>44595</v>
       </c>
-      <c r="B189" s="5">
+      <c r="B189">
         <v>29</v>
       </c>
-      <c r="C189" s="5">
-        <v>5</v>
+      <c r="C189">
+        <v>2</v>
       </c>
       <c r="D189" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E189" s="5">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F189" s="5">
-        <v>7.0000000000000007E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="G189" s="5">
-        <v>12.5</v>
+        <v>25</v>
       </c>
       <c r="H189" s="5">
         <v>0</v>
       </c>
       <c r="I189" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="6">
         <v>44595</v>
       </c>
-      <c r="B190" s="5">
+      <c r="B190">
         <v>29</v>
       </c>
-      <c r="C190" s="5">
-        <v>8</v>
+      <c r="C190">
+        <v>3</v>
       </c>
       <c r="D190" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E190" s="5">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F190" s="5">
-        <v>3.5000000000000003E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G190" s="5">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="H190" s="5">
         <v>0</v>
       </c>
       <c r="I190" s="5" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
@@ -6120,25 +6125,25 @@
         <v>29</v>
       </c>
       <c r="C191" s="5">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D191" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E191" s="5">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F191" s="5">
-        <v>7.0000000000000007E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="G191" s="5">
-        <v>12.5</v>
+        <v>25</v>
       </c>
       <c r="H191" s="5">
         <v>0</v>
       </c>
       <c r="I191" s="5" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
@@ -6149,7 +6154,7 @@
         <v>29</v>
       </c>
       <c r="C192" s="5">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D192" s="5" t="s">
         <v>5</v>
@@ -6177,8 +6182,8 @@
       <c r="B193" s="5">
         <v>29</v>
       </c>
-      <c r="C193" s="5">
-        <v>13</v>
+      <c r="C193">
+        <v>6</v>
       </c>
       <c r="D193" s="5" t="s">
         <v>5</v>
@@ -6195,8 +6200,8 @@
       <c r="H193" s="5">
         <v>0</v>
       </c>
-      <c r="I193" s="5" t="s">
-        <v>44</v>
+      <c r="I193" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
@@ -6206,26 +6211,26 @@
       <c r="B194" s="5">
         <v>29</v>
       </c>
-      <c r="C194" s="5">
-        <v>14</v>
+      <c r="C194">
+        <v>7</v>
       </c>
       <c r="D194" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E194" s="5">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="F194" s="5">
-        <v>0.7</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G194" s="5">
-        <v>1.25</v>
+        <v>12.5</v>
       </c>
       <c r="H194" s="5">
         <v>0</v>
       </c>
-      <c r="I194" s="5" t="s">
-        <v>31</v>
+      <c r="I194" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
@@ -6236,24 +6241,169 @@
         <v>29</v>
       </c>
       <c r="C195" s="5">
+        <v>8</v>
+      </c>
+      <c r="D195" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E195" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F195" s="5">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G195" s="5">
+        <v>25</v>
+      </c>
+      <c r="H195" s="5">
+        <v>0</v>
+      </c>
+      <c r="I195" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A196" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B196" s="5">
+        <v>29</v>
+      </c>
+      <c r="C196" s="5">
+        <v>9</v>
+      </c>
+      <c r="D196" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E196" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F196" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G196" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="H196" s="5">
+        <v>0</v>
+      </c>
+      <c r="I196" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B197" s="5">
+        <v>29</v>
+      </c>
+      <c r="C197" s="5">
+        <v>12</v>
+      </c>
+      <c r="D197" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E197" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F197" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G197" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="H197" s="5">
+        <v>0</v>
+      </c>
+      <c r="I197" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A198" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B198" s="5">
+        <v>29</v>
+      </c>
+      <c r="C198" s="5">
+        <v>13</v>
+      </c>
+      <c r="D198" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E198" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F198" s="5">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G198" s="5">
+        <v>25</v>
+      </c>
+      <c r="H198" s="5">
+        <v>0</v>
+      </c>
+      <c r="I198" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B199" s="5">
+        <v>29</v>
+      </c>
+      <c r="C199" s="5">
+        <v>14</v>
+      </c>
+      <c r="D199" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E199" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F199" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="G199" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="H199" s="5">
+        <v>0</v>
+      </c>
+      <c r="I199" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B200" s="5">
+        <v>29</v>
+      </c>
+      <c r="C200" s="5">
         <v>15</v>
       </c>
-      <c r="D195" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E195" s="5">
+      <c r="D200" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E200" s="5">
         <v>0.1</v>
       </c>
-      <c r="F195" s="5">
+      <c r="F200" s="5">
         <v>0.7</v>
       </c>
-      <c r="G195" s="5">
+      <c r="G200" s="5">
         <v>1.25</v>
       </c>
-      <c r="H195" s="5">
-        <v>0</v>
-      </c>
-      <c r="I195" s="5" t="s">
+      <c r="H200" s="5">
+        <v>0</v>
+      </c>
+      <c r="I200" s="5" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
badLOC detection and outlier message
</commit_message>
<xml_diff>
--- a/fly_record.xlsx
+++ b/fly_record.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\group_swinderen\Bruno\Sequential Effects ERP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\group_swinderen\Dinis\Sequential Effects ERP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B429F78-48B1-40A6-A3DF-2FB38AD3A630}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAFAA29-0820-4B6B-8E61-B97E0DEFE056}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10800" windowHeight="5190" xr2:uid="{0C11348E-E482-4597-B3FE-1374AFB87193}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -178,6 +178,18 @@
       <t>2 LFP channels: ch1 CX, ch2, OL</t>
     </r>
   </si>
+  <si>
+    <t>baseline, regular</t>
+  </si>
+  <si>
+    <t>jittering</t>
+  </si>
+  <si>
+    <t>regular</t>
+  </si>
+  <si>
+    <t>alternating to calibrate</t>
+  </si>
 </sst>
 </file>
 
@@ -223,12 +235,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680E0717-9BF1-4D4C-A430-96F9A20E59A5}">
-  <dimension ref="A1:I183"/>
+  <dimension ref="A1:I200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="I149" sqref="I149"/>
+    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
+      <selection activeCell="F197" sqref="F197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5900,6 +5914,499 @@
         <v>31</v>
       </c>
     </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>44594</v>
+      </c>
+      <c r="B184">
+        <v>28</v>
+      </c>
+      <c r="C184">
+        <v>7</v>
+      </c>
+      <c r="D184" t="s">
+        <v>5</v>
+      </c>
+      <c r="E184">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F184">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G184">
+        <v>25</v>
+      </c>
+      <c r="H184">
+        <v>0</v>
+      </c>
+      <c r="I184" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>44594</v>
+      </c>
+      <c r="B185">
+        <v>28</v>
+      </c>
+      <c r="C185">
+        <v>8</v>
+      </c>
+      <c r="D185" t="s">
+        <v>5</v>
+      </c>
+      <c r="E185">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F185">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G185">
+        <v>25</v>
+      </c>
+      <c r="H185">
+        <v>0</v>
+      </c>
+      <c r="I185" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>44594</v>
+      </c>
+      <c r="B186">
+        <v>28</v>
+      </c>
+      <c r="C186">
+        <v>9</v>
+      </c>
+      <c r="D186" t="s">
+        <v>5</v>
+      </c>
+      <c r="E186">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F186">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G186">
+        <v>25</v>
+      </c>
+      <c r="H186">
+        <v>0</v>
+      </c>
+      <c r="I186" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A187" s="6">
+        <v>44594</v>
+      </c>
+      <c r="B187" s="5">
+        <v>28</v>
+      </c>
+      <c r="C187" s="5">
+        <v>10</v>
+      </c>
+      <c r="D187" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E187" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F187" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G187" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="H187" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A188" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B188">
+        <v>29</v>
+      </c>
+      <c r="C188">
+        <v>1</v>
+      </c>
+      <c r="D188" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E188" s="5">
+        <f>1*1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F188" s="5">
+        <f>4*1/200</f>
+        <v>0.02</v>
+      </c>
+      <c r="G188" s="5">
+        <f t="shared" ref="G188" si="18">1/(E188+F188)</f>
+        <v>40</v>
+      </c>
+      <c r="H188" s="5">
+        <v>0</v>
+      </c>
+      <c r="I188" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A189" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B189">
+        <v>29</v>
+      </c>
+      <c r="C189">
+        <v>2</v>
+      </c>
+      <c r="D189" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E189" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F189" s="5">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G189" s="5">
+        <v>25</v>
+      </c>
+      <c r="H189" s="5">
+        <v>0</v>
+      </c>
+      <c r="I189" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A190" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B190">
+        <v>29</v>
+      </c>
+      <c r="C190">
+        <v>3</v>
+      </c>
+      <c r="D190" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E190" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F190" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G190" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="H190" s="5">
+        <v>0</v>
+      </c>
+      <c r="I190" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A191" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B191" s="5">
+        <v>29</v>
+      </c>
+      <c r="C191" s="5">
+        <v>4</v>
+      </c>
+      <c r="D191" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E191" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F191" s="5">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G191" s="5">
+        <v>25</v>
+      </c>
+      <c r="H191" s="5">
+        <v>0</v>
+      </c>
+      <c r="I191" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A192" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B192" s="5">
+        <v>29</v>
+      </c>
+      <c r="C192" s="5">
+        <v>5</v>
+      </c>
+      <c r="D192" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E192" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F192" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G192" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="H192" s="5">
+        <v>0</v>
+      </c>
+      <c r="I192" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A193" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B193" s="5">
+        <v>29</v>
+      </c>
+      <c r="C193">
+        <v>6</v>
+      </c>
+      <c r="D193" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E193" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F193" s="5">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G193" s="5">
+        <v>25</v>
+      </c>
+      <c r="H193" s="5">
+        <v>0</v>
+      </c>
+      <c r="I193" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A194" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B194" s="5">
+        <v>29</v>
+      </c>
+      <c r="C194">
+        <v>7</v>
+      </c>
+      <c r="D194" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E194" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F194" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G194" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="H194" s="5">
+        <v>0</v>
+      </c>
+      <c r="I194" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A195" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B195" s="5">
+        <v>29</v>
+      </c>
+      <c r="C195" s="5">
+        <v>8</v>
+      </c>
+      <c r="D195" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E195" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F195" s="5">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G195" s="5">
+        <v>25</v>
+      </c>
+      <c r="H195" s="5">
+        <v>0</v>
+      </c>
+      <c r="I195" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A196" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B196" s="5">
+        <v>29</v>
+      </c>
+      <c r="C196" s="5">
+        <v>9</v>
+      </c>
+      <c r="D196" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E196" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F196" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G196" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="H196" s="5">
+        <v>0</v>
+      </c>
+      <c r="I196" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B197" s="5">
+        <v>29</v>
+      </c>
+      <c r="C197" s="5">
+        <v>12</v>
+      </c>
+      <c r="D197" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E197" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F197" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G197" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="H197" s="5">
+        <v>0</v>
+      </c>
+      <c r="I197" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A198" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B198" s="5">
+        <v>29</v>
+      </c>
+      <c r="C198" s="5">
+        <v>13</v>
+      </c>
+      <c r="D198" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E198" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F198" s="5">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G198" s="5">
+        <v>25</v>
+      </c>
+      <c r="H198" s="5">
+        <v>0</v>
+      </c>
+      <c r="I198" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B199" s="5">
+        <v>29</v>
+      </c>
+      <c r="C199" s="5">
+        <v>14</v>
+      </c>
+      <c r="D199" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E199" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F199" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="G199" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="H199" s="5">
+        <v>0</v>
+      </c>
+      <c r="I199" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200" s="6">
+        <v>44595</v>
+      </c>
+      <c r="B200" s="5">
+        <v>29</v>
+      </c>
+      <c r="C200" s="5">
+        <v>15</v>
+      </c>
+      <c r="D200" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E200" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F200" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="G200" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="H200" s="5">
+        <v>0</v>
+      </c>
+      <c r="I200" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added exponential filter fits
</commit_message>
<xml_diff>
--- a/fly_record.xlsx
+++ b/fly_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\group_swinderen\Dinis\Sequential Effects ERP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DE89B2-C3D0-4D50-B850-C18D6FA45153}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3133B5-241F-4BA9-8884-7595E7174769}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10800" windowHeight="5190" xr2:uid="{0C11348E-E482-4597-B3FE-1374AFB87193}"/>
   </bookViews>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680E0717-9BF1-4D4C-A430-96F9A20E59A5}">
   <dimension ref="A1:L200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="J184" sqref="J184"/>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="I185" sqref="I185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4770,10 +4770,10 @@
         <v>0</v>
       </c>
       <c r="I132" s="5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J132" s="5">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K132" s="5">
         <v>0.4</v>
@@ -5360,10 +5360,10 @@
         <v>0</v>
       </c>
       <c r="I149" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="J149" s="5">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="K149" s="5">
         <v>0.1</v>
@@ -5498,7 +5498,7 @@
         <v>0</v>
       </c>
       <c r="I153" s="5">
-        <v>-1.5</v>
+        <v>-2</v>
       </c>
       <c r="J153" s="5">
         <v>1.3</v>
@@ -5703,10 +5703,10 @@
         <v>0</v>
       </c>
       <c r="I159" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="J159" s="5">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="K159" s="5">
         <v>0.4</v>
@@ -6155,13 +6155,13 @@
         <v>0</v>
       </c>
       <c r="I171" s="5">
-        <v>-1.5</v>
+        <v>0</v>
       </c>
       <c r="J171" s="5">
-        <v>1.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K171" s="5">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="L171" t="s">
         <v>40</v>
@@ -6224,10 +6224,10 @@
         <v>0</v>
       </c>
       <c r="I173" s="5">
-        <v>0</v>
+        <v>-1.5</v>
       </c>
       <c r="J173" s="5">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="K173" s="5">
         <v>0.4</v>
@@ -6436,10 +6436,10 @@
         <v>0</v>
       </c>
       <c r="I179" s="5">
-        <v>0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="J179" s="5">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="K179" s="5">
         <v>0.4</v>
@@ -6616,7 +6616,7 @@
         <v>0</v>
       </c>
       <c r="I184" s="5">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="J184" s="5">
         <v>1.1000000000000001</v>

</xml_diff>

<commit_message>
Added and corrected block analysis
</commit_message>
<xml_diff>
--- a/fly_record.xlsx
+++ b/fly_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\group_swinderen\Dinis\Sequential Effects ERP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A4C815-9A91-4B8A-B59D-7CD3514FAE27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07071427-AE0C-4304-BF19-1CBE55474957}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10800" windowHeight="5190" xr2:uid="{0C11348E-E482-4597-B3FE-1374AFB87193}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -243,6 +243,24 @@
   </si>
   <si>
     <t>regular, front, no ATR</t>
+  </si>
+  <si>
+    <t>regular, front, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular, sides, no ATR, blue</t>
+  </si>
+  <si>
+    <t>blocks, front, blue</t>
+  </si>
+  <si>
+    <t>blocks, sides, blue</t>
+  </si>
+  <si>
+    <t>InterBlockPeriod</t>
+  </si>
+  <si>
+    <t>BlockLength</t>
   </si>
 </sst>
 </file>
@@ -611,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680E0717-9BF1-4D4C-A430-96F9A20E59A5}">
-  <dimension ref="A1:L257"/>
+  <dimension ref="A1:N276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="L247" sqref="L247"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="K194" sqref="K194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,10 +641,12 @@
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="84.140625" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="84.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -661,10 +681,16 @@
         <v>46</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44489</v>
       </c>
@@ -699,7 +725,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44489</v>
       </c>
@@ -725,7 +751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44489</v>
       </c>
@@ -760,7 +786,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44489</v>
       </c>
@@ -786,7 +812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44491</v>
       </c>
@@ -821,7 +847,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44491</v>
       </c>
@@ -847,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44491</v>
       </c>
@@ -882,7 +908,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44491</v>
       </c>
@@ -917,7 +943,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44491</v>
       </c>
@@ -943,7 +969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44495</v>
       </c>
@@ -978,7 +1004,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44495</v>
       </c>
@@ -1003,11 +1029,11 @@
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44497</v>
       </c>
@@ -1042,7 +1068,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44497</v>
       </c>
@@ -1068,7 +1094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44497</v>
       </c>
@@ -1102,11 +1128,11 @@
       <c r="K15" s="5">
         <v>0.4</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44497</v>
       </c>
@@ -1140,11 +1166,11 @@
       <c r="K16" s="5">
         <v>0.4</v>
       </c>
-      <c r="L16" t="s">
+      <c r="N16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44497</v>
       </c>
@@ -1169,11 +1195,11 @@
       <c r="H17" s="4">
         <v>1</v>
       </c>
-      <c r="L17" t="s">
+      <c r="N17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44503</v>
       </c>
@@ -1208,7 +1234,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44503</v>
       </c>
@@ -1234,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44503</v>
       </c>
@@ -1269,7 +1295,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44503</v>
       </c>
@@ -1304,7 +1330,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44503</v>
       </c>
@@ -1329,11 +1355,11 @@
       <c r="H22" s="4">
         <v>0</v>
       </c>
-      <c r="L22" t="s">
+      <c r="N22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44509</v>
       </c>
@@ -1359,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44509</v>
       </c>
@@ -1394,7 +1420,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44509</v>
       </c>
@@ -1423,7 +1449,7 @@
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44509</v>
       </c>
@@ -1449,7 +1475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44509</v>
       </c>
@@ -1484,7 +1510,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44509</v>
       </c>
@@ -1510,7 +1536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44512</v>
       </c>
@@ -1545,7 +1571,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44512</v>
       </c>
@@ -1571,7 +1597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44512</v>
       </c>
@@ -1605,11 +1631,11 @@
       <c r="K31" s="5">
         <v>0.4</v>
       </c>
-      <c r="L31" t="s">
+      <c r="N31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44512</v>
       </c>
@@ -1635,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44512</v>
       </c>
@@ -1670,7 +1696,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44512</v>
       </c>
@@ -1695,11 +1721,11 @@
       <c r="H34" s="4">
         <v>1</v>
       </c>
-      <c r="L34" t="s">
+      <c r="N34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44512</v>
       </c>
@@ -1725,7 +1751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44512</v>
       </c>
@@ -1751,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44518</v>
       </c>
@@ -1779,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44518</v>
       </c>
@@ -1807,7 +1833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44518</v>
       </c>
@@ -1835,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44518</v>
       </c>
@@ -1863,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44518</v>
       </c>
@@ -1890,11 +1916,11 @@
       <c r="H41" s="4">
         <v>0</v>
       </c>
-      <c r="L41" t="s">
+      <c r="N41" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44518</v>
       </c>
@@ -1921,11 +1947,11 @@
       <c r="H42" s="4">
         <v>0</v>
       </c>
-      <c r="L42" t="s">
+      <c r="N42" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44518</v>
       </c>
@@ -1953,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44518</v>
       </c>
@@ -1980,11 +2006,11 @@
       <c r="H44" s="4">
         <v>0</v>
       </c>
-      <c r="L44" t="s">
+      <c r="N44" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44518</v>
       </c>
@@ -2009,11 +2035,11 @@
       <c r="H45" s="4">
         <v>1</v>
       </c>
-      <c r="L45" t="s">
+      <c r="N45" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44518</v>
       </c>
@@ -2041,7 +2067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44518</v>
       </c>
@@ -2069,7 +2095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44518</v>
       </c>
@@ -2097,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44518</v>
       </c>
@@ -2125,7 +2151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44518</v>
       </c>
@@ -2152,11 +2178,11 @@
       <c r="H50" s="4">
         <v>0</v>
       </c>
-      <c r="L50" t="s">
+      <c r="N50" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44518</v>
       </c>
@@ -2183,11 +2209,11 @@
       <c r="H51" s="4">
         <v>0</v>
       </c>
-      <c r="L51" t="s">
+      <c r="N51" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44519</v>
       </c>
@@ -2212,11 +2238,11 @@
       <c r="H52" s="4">
         <v>1</v>
       </c>
-      <c r="L52" t="s">
+      <c r="N52" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44519</v>
       </c>
@@ -2241,11 +2267,11 @@
       <c r="H53" s="4">
         <v>1</v>
       </c>
-      <c r="L53" t="s">
+      <c r="N53" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44525</v>
       </c>
@@ -2272,11 +2298,11 @@
       <c r="H54" s="4">
         <v>0</v>
       </c>
-      <c r="L54" t="s">
+      <c r="N54" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44525</v>
       </c>
@@ -2303,11 +2329,11 @@
       <c r="H55" s="4">
         <v>0</v>
       </c>
-      <c r="L55" t="s">
+      <c r="N55" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44525</v>
       </c>
@@ -2334,11 +2360,11 @@
       <c r="H56" s="4">
         <v>0</v>
       </c>
-      <c r="L56" t="s">
+      <c r="N56" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44525</v>
       </c>
@@ -2365,11 +2391,11 @@
       <c r="H57" s="4">
         <v>0</v>
       </c>
-      <c r="L57" t="s">
+      <c r="N57" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44525</v>
       </c>
@@ -2396,11 +2422,11 @@
       <c r="H58" s="4">
         <v>0</v>
       </c>
-      <c r="L58" t="s">
+      <c r="N58" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44525</v>
       </c>
@@ -2427,11 +2453,11 @@
       <c r="H59" s="4">
         <v>0</v>
       </c>
-      <c r="L59" t="s">
+      <c r="N59" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44525</v>
       </c>
@@ -2456,11 +2482,11 @@
       <c r="H60" s="4">
         <v>1</v>
       </c>
-      <c r="L60" s="4" t="s">
+      <c r="N60" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44525</v>
       </c>
@@ -2485,11 +2511,11 @@
       <c r="H61" s="4">
         <v>1</v>
       </c>
-      <c r="L61" t="s">
+      <c r="N61" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44525</v>
       </c>
@@ -2516,11 +2542,11 @@
       <c r="H62" s="4">
         <v>1</v>
       </c>
-      <c r="L62" t="s">
+      <c r="N62" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44525</v>
       </c>
@@ -2547,11 +2573,11 @@
       <c r="H63" s="4">
         <v>1</v>
       </c>
-      <c r="L63" t="s">
+      <c r="N63" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44525</v>
       </c>
@@ -2578,11 +2604,11 @@
       <c r="H64" s="4">
         <v>1</v>
       </c>
-      <c r="L64" t="s">
+      <c r="N64" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44525</v>
       </c>
@@ -2609,11 +2635,11 @@
       <c r="H65" s="4">
         <v>1</v>
       </c>
-      <c r="L65" t="s">
+      <c r="N65" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44525</v>
       </c>
@@ -2640,11 +2666,11 @@
       <c r="H66" s="4">
         <v>1</v>
       </c>
-      <c r="L66" t="s">
+      <c r="N66" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44525</v>
       </c>
@@ -2671,11 +2697,11 @@
       <c r="H67" s="4">
         <v>1</v>
       </c>
-      <c r="L67" t="s">
+      <c r="N67" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44532</v>
       </c>
@@ -2704,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44532</v>
       </c>
@@ -2733,7 +2759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44532</v>
       </c>
@@ -2771,7 +2797,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44532</v>
       </c>
@@ -2800,7 +2826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44532</v>
       </c>
@@ -2838,7 +2864,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44532</v>
       </c>
@@ -2867,7 +2893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44532</v>
       </c>
@@ -2905,7 +2931,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44532</v>
       </c>
@@ -2934,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44532</v>
       </c>
@@ -2972,7 +2998,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44532</v>
       </c>
@@ -3001,7 +3027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44532</v>
       </c>
@@ -3030,7 +3056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44532</v>
       </c>
@@ -3059,7 +3085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44538</v>
       </c>
@@ -3097,7 +3123,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44538</v>
       </c>
@@ -3126,7 +3152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44538</v>
       </c>
@@ -3164,7 +3190,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44538</v>
       </c>
@@ -3193,7 +3219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44538</v>
       </c>
@@ -3231,7 +3257,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44538</v>
       </c>
@@ -3260,7 +3286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44538</v>
       </c>
@@ -3289,7 +3315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44538</v>
       </c>
@@ -3318,7 +3344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44538</v>
       </c>
@@ -3347,7 +3373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44538</v>
       </c>
@@ -3376,7 +3402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44538</v>
       </c>
@@ -3413,11 +3439,11 @@
       <c r="K90" s="5">
         <v>0.4</v>
       </c>
-      <c r="L90" t="s">
+      <c r="N90" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44538</v>
       </c>
@@ -3446,7 +3472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44538</v>
       </c>
@@ -3484,7 +3510,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44538</v>
       </c>
@@ -3513,7 +3539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44538</v>
       </c>
@@ -3551,7 +3577,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44538</v>
       </c>
@@ -3580,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44538</v>
       </c>
@@ -3618,7 +3644,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44538</v>
       </c>
@@ -3647,7 +3673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44538</v>
       </c>
@@ -3676,7 +3702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44538</v>
       </c>
@@ -3705,7 +3731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44538</v>
       </c>
@@ -3734,7 +3760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44538</v>
       </c>
@@ -3763,7 +3789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44547</v>
       </c>
@@ -3800,11 +3826,11 @@
       <c r="K102" s="5">
         <v>0.4</v>
       </c>
-      <c r="L102" t="s">
+      <c r="N102" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44547</v>
       </c>
@@ -3832,11 +3858,11 @@
       <c r="H103" s="4">
         <v>0</v>
       </c>
-      <c r="L103" s="4" t="s">
+      <c r="N103" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44547</v>
       </c>
@@ -3873,11 +3899,11 @@
       <c r="K104" s="5">
         <v>0.4</v>
       </c>
-      <c r="L104" s="4" t="s">
+      <c r="N104" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44547</v>
       </c>
@@ -3905,11 +3931,11 @@
       <c r="H105" s="4">
         <v>0</v>
       </c>
-      <c r="L105" s="4" t="s">
+      <c r="N105" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44547</v>
       </c>
@@ -3946,11 +3972,11 @@
       <c r="K106" s="5">
         <v>0.4</v>
       </c>
-      <c r="L106" s="4" t="s">
+      <c r="N106" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44547</v>
       </c>
@@ -3978,11 +4004,11 @@
       <c r="H107" s="4">
         <v>0</v>
       </c>
-      <c r="L107" s="4" t="s">
+      <c r="N107" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44547</v>
       </c>
@@ -4010,11 +4036,11 @@
       <c r="H108" s="4">
         <v>0</v>
       </c>
-      <c r="L108" s="4" t="s">
+      <c r="N108" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44547</v>
       </c>
@@ -4042,11 +4068,11 @@
       <c r="H109" s="4">
         <v>0</v>
       </c>
-      <c r="L109" s="4" t="s">
+      <c r="N109" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44547</v>
       </c>
@@ -4074,11 +4100,11 @@
       <c r="H110" s="4">
         <v>0</v>
       </c>
-      <c r="L110" s="4" t="s">
+      <c r="N110" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44547</v>
       </c>
@@ -4106,11 +4132,11 @@
       <c r="H111" s="4">
         <v>0</v>
       </c>
-      <c r="L111" s="4" t="s">
+      <c r="N111" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44547</v>
       </c>
@@ -4147,11 +4173,11 @@
       <c r="K112" s="5">
         <v>0.4</v>
       </c>
-      <c r="L112" s="4" t="s">
+      <c r="N112" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44547</v>
       </c>
@@ -4179,11 +4205,11 @@
       <c r="H113" s="4">
         <v>0</v>
       </c>
-      <c r="L113" s="4" t="s">
+      <c r="N113" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44552</v>
       </c>
@@ -4220,11 +4246,11 @@
       <c r="K114" s="5">
         <v>0.4</v>
       </c>
-      <c r="L114" t="s">
+      <c r="N114" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44552</v>
       </c>
@@ -4253,7 +4279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44552</v>
       </c>
@@ -4291,7 +4317,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44552</v>
       </c>
@@ -4320,7 +4346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44552</v>
       </c>
@@ -4358,7 +4384,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44552</v>
       </c>
@@ -4387,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44552</v>
       </c>
@@ -4425,7 +4451,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44552</v>
       </c>
@@ -4454,7 +4480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44552</v>
       </c>
@@ -4483,7 +4509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44552</v>
       </c>
@@ -4512,7 +4538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44552</v>
       </c>
@@ -4541,7 +4567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44552</v>
       </c>
@@ -4570,7 +4596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44575</v>
       </c>
@@ -4604,11 +4630,11 @@
       <c r="K126" s="5">
         <v>0.4</v>
       </c>
-      <c r="L126" t="s">
+      <c r="N126" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44575</v>
       </c>
@@ -4633,11 +4659,11 @@
       <c r="H127">
         <v>0</v>
       </c>
-      <c r="L127" t="s">
+      <c r="N127" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44575</v>
       </c>
@@ -4673,11 +4699,11 @@
       <c r="K128" s="5">
         <v>0.4</v>
       </c>
-      <c r="L128" t="s">
+      <c r="N128" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44575</v>
       </c>
@@ -4704,11 +4730,11 @@
       <c r="H129" s="4">
         <v>0</v>
       </c>
-      <c r="L129" t="s">
+      <c r="N129" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44575</v>
       </c>
@@ -4742,11 +4768,11 @@
       <c r="K130" s="5">
         <v>0.4</v>
       </c>
-      <c r="L130" t="s">
+      <c r="N130" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44575</v>
       </c>
@@ -4771,11 +4797,11 @@
       <c r="H131" s="4">
         <v>0</v>
       </c>
-      <c r="L131" t="s">
+      <c r="N131" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>44575</v>
       </c>
@@ -4811,11 +4837,11 @@
       <c r="K132" s="5">
         <v>0.4</v>
       </c>
-      <c r="L132" s="4" t="s">
+      <c r="N132" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44575</v>
       </c>
@@ -4849,11 +4875,11 @@
       <c r="K133" s="5">
         <v>0.4</v>
       </c>
-      <c r="L133" s="4" t="s">
+      <c r="N133" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44575</v>
       </c>
@@ -4878,11 +4904,11 @@
       <c r="H134">
         <v>0</v>
       </c>
-      <c r="L134" t="s">
+      <c r="N134" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44575</v>
       </c>
@@ -4918,11 +4944,11 @@
       <c r="K135" s="5">
         <v>0.1</v>
       </c>
-      <c r="L135" t="s">
+      <c r="N135" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44575</v>
       </c>
@@ -4949,11 +4975,11 @@
       <c r="H136" s="4">
         <v>0</v>
       </c>
-      <c r="L136" t="s">
+      <c r="N136" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44575</v>
       </c>
@@ -4987,11 +5013,11 @@
       <c r="K137" s="5">
         <v>0.1</v>
       </c>
-      <c r="L137" t="s">
+      <c r="N137" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44575</v>
       </c>
@@ -5016,11 +5042,11 @@
       <c r="H138" s="4">
         <v>0</v>
       </c>
-      <c r="L138" t="s">
+      <c r="N138" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44575</v>
       </c>
@@ -5056,11 +5082,11 @@
       <c r="K139" s="5">
         <v>0.1</v>
       </c>
-      <c r="L139" t="s">
+      <c r="N139" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44575</v>
       </c>
@@ -5087,11 +5113,11 @@
       <c r="H140" s="4">
         <v>0</v>
       </c>
-      <c r="L140" t="s">
+      <c r="N140" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44575</v>
       </c>
@@ -5125,11 +5151,11 @@
       <c r="K141" s="5">
         <v>0.1</v>
       </c>
-      <c r="L141" t="s">
+      <c r="N141" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44575</v>
       </c>
@@ -5154,11 +5180,11 @@
       <c r="H142" s="4">
         <v>0</v>
       </c>
-      <c r="L142" t="s">
+      <c r="N142" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44575</v>
       </c>
@@ -5185,11 +5211,11 @@
       <c r="H143" s="4">
         <v>0</v>
       </c>
-      <c r="L143" t="s">
+      <c r="N143" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44575</v>
       </c>
@@ -5225,11 +5251,11 @@
       <c r="K144" s="5">
         <v>0.4</v>
       </c>
-      <c r="L144" t="s">
+      <c r="N144" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44575</v>
       </c>
@@ -5263,11 +5289,11 @@
       <c r="K145" s="5">
         <v>0.1</v>
       </c>
-      <c r="L145" t="s">
+      <c r="N145" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44575</v>
       </c>
@@ -5292,11 +5318,11 @@
       <c r="H146" s="4">
         <v>0</v>
       </c>
-      <c r="L146" t="s">
+      <c r="N146" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44575</v>
       </c>
@@ -5332,11 +5358,11 @@
       <c r="K147" s="5">
         <v>0.1</v>
       </c>
-      <c r="L147" t="s">
+      <c r="N147" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44575</v>
       </c>
@@ -5363,11 +5389,11 @@
       <c r="H148" s="4">
         <v>0</v>
       </c>
-      <c r="L148" t="s">
+      <c r="N148" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44580</v>
       </c>
@@ -5401,11 +5427,11 @@
       <c r="K149" s="5">
         <v>0.1</v>
       </c>
-      <c r="L149" t="s">
+      <c r="N149" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44580</v>
       </c>
@@ -5430,11 +5456,11 @@
       <c r="H150" s="4">
         <v>0</v>
       </c>
-      <c r="L150" t="s">
+      <c r="N150" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44580</v>
       </c>
@@ -5470,11 +5496,11 @@
       <c r="K151" s="5">
         <v>0.1</v>
       </c>
-      <c r="L151" t="s">
+      <c r="N151" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44580</v>
       </c>
@@ -5501,11 +5527,11 @@
       <c r="H152" s="4">
         <v>0</v>
       </c>
-      <c r="L152" t="s">
+      <c r="N152" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44580</v>
       </c>
@@ -5539,11 +5565,11 @@
       <c r="K153" s="5">
         <v>0.4</v>
       </c>
-      <c r="L153" t="s">
+      <c r="N153" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44580</v>
       </c>
@@ -5568,11 +5594,11 @@
       <c r="H154" s="4">
         <v>0</v>
       </c>
-      <c r="L154" t="s">
+      <c r="N154" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44580</v>
       </c>
@@ -5606,11 +5632,11 @@
       <c r="K155" s="5">
         <v>0.4</v>
       </c>
-      <c r="L155" t="s">
+      <c r="N155" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44580</v>
       </c>
@@ -5646,11 +5672,11 @@
       <c r="K156" s="5">
         <v>0.4</v>
       </c>
-      <c r="L156" t="s">
+      <c r="N156" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44580</v>
       </c>
@@ -5677,11 +5703,11 @@
       <c r="H157" s="4">
         <v>0</v>
       </c>
-      <c r="L157" t="s">
+      <c r="N157" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44580</v>
       </c>
@@ -5706,11 +5732,11 @@
       <c r="H158" s="4">
         <v>0</v>
       </c>
-      <c r="L158" s="4" t="s">
+      <c r="N158" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44580</v>
       </c>
@@ -5744,11 +5770,11 @@
       <c r="K159" s="5">
         <v>0.4</v>
       </c>
-      <c r="L159" t="s">
+      <c r="N159" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44580</v>
       </c>
@@ -5773,11 +5799,11 @@
       <c r="H160" s="4">
         <v>0</v>
       </c>
-      <c r="L160" t="s">
+      <c r="N160" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44580</v>
       </c>
@@ -5804,11 +5830,11 @@
       <c r="H161" s="4">
         <v>0</v>
       </c>
-      <c r="L161" t="s">
+      <c r="N161" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44580</v>
       </c>
@@ -5844,11 +5870,11 @@
       <c r="K162" s="5">
         <v>0.1</v>
       </c>
-      <c r="L162" t="s">
+      <c r="N162" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44580</v>
       </c>
@@ -5882,11 +5908,11 @@
       <c r="K163" s="5">
         <v>0.4</v>
       </c>
-      <c r="L163" t="s">
+      <c r="N163" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44580</v>
       </c>
@@ -5922,11 +5948,11 @@
       <c r="K164" s="5">
         <v>0.1</v>
       </c>
-      <c r="L164" s="4" t="s">
+      <c r="N164" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44580</v>
       </c>
@@ -5962,11 +5988,11 @@
       <c r="K165" s="5">
         <v>0.4</v>
       </c>
-      <c r="L165" s="4" t="s">
+      <c r="N165" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44580</v>
       </c>
@@ -6000,11 +6026,11 @@
       <c r="K166" s="5">
         <v>0.4</v>
       </c>
-      <c r="L166" s="4" t="s">
+      <c r="N166" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44580</v>
       </c>
@@ -6038,11 +6064,11 @@
       <c r="K167" s="5">
         <v>0.4</v>
       </c>
-      <c r="L167" s="4" t="s">
+      <c r="N167" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44580</v>
       </c>
@@ -6078,11 +6104,11 @@
       <c r="K168" s="5">
         <v>0.1</v>
       </c>
-      <c r="L168" s="4" t="s">
+      <c r="N168" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44580</v>
       </c>
@@ -6118,11 +6144,11 @@
       <c r="K169" s="5">
         <v>0.4</v>
       </c>
-      <c r="L169" s="4" t="s">
+      <c r="N169" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44580</v>
       </c>
@@ -6156,11 +6182,11 @@
       <c r="K170" s="5">
         <v>0.4</v>
       </c>
-      <c r="L170" s="4" t="s">
+      <c r="N170" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44581</v>
       </c>
@@ -6196,11 +6222,11 @@
       <c r="K171" s="5">
         <v>0.4</v>
       </c>
-      <c r="L171" t="s">
+      <c r="N171" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44581</v>
       </c>
@@ -6227,11 +6253,11 @@
       <c r="H172" s="4">
         <v>0</v>
       </c>
-      <c r="L172" t="s">
+      <c r="N172" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44581</v>
       </c>
@@ -6265,11 +6291,11 @@
       <c r="K173" s="5">
         <v>0.4</v>
       </c>
-      <c r="L173" t="s">
+      <c r="N173" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44581</v>
       </c>
@@ -6294,11 +6320,11 @@
       <c r="H174" s="4">
         <v>0</v>
       </c>
-      <c r="L174" t="s">
+      <c r="N174" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44581</v>
       </c>
@@ -6332,11 +6358,11 @@
       <c r="K175" s="5">
         <v>0.4</v>
       </c>
-      <c r="L175" t="s">
+      <c r="N175" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44581</v>
       </c>
@@ -6361,11 +6387,11 @@
       <c r="H176" s="4">
         <v>0</v>
       </c>
-      <c r="L176" t="s">
+      <c r="N176" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>44581</v>
       </c>
@@ -6399,11 +6425,11 @@
       <c r="K177" s="5">
         <v>0.4</v>
       </c>
-      <c r="L177" t="s">
+      <c r="N177" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>44581</v>
       </c>
@@ -6439,11 +6465,11 @@
       <c r="K178" s="5">
         <v>0.4</v>
       </c>
-      <c r="L178" t="s">
+      <c r="N178" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>44581</v>
       </c>
@@ -6477,11 +6503,11 @@
       <c r="K179" s="5">
         <v>0.4</v>
       </c>
-      <c r="L179" t="s">
+      <c r="N179" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>44581</v>
       </c>
@@ -6517,11 +6543,11 @@
       <c r="K180" s="5">
         <v>0.4</v>
       </c>
-      <c r="L180" t="s">
+      <c r="N180" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>44581</v>
       </c>
@@ -6546,11 +6572,11 @@
       <c r="H181" s="4">
         <v>0</v>
       </c>
-      <c r="L181" t="s">
+      <c r="N181" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>44581</v>
       </c>
@@ -6578,11 +6604,11 @@
       <c r="H182" s="4">
         <v>0</v>
       </c>
-      <c r="L182" t="s">
+      <c r="N182" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>44581</v>
       </c>
@@ -6619,11 +6645,11 @@
       <c r="K183" s="5">
         <v>0.4</v>
       </c>
-      <c r="L183" t="s">
+      <c r="N183" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>44594</v>
       </c>
@@ -6657,11 +6683,11 @@
       <c r="K184" s="5">
         <v>0.4</v>
       </c>
-      <c r="L184" t="s">
+      <c r="N184" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>44594</v>
       </c>
@@ -6695,11 +6721,11 @@
       <c r="K185" s="5">
         <v>0.4</v>
       </c>
-      <c r="L185" t="s">
+      <c r="N185" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>44594</v>
       </c>
@@ -6733,11 +6759,11 @@
       <c r="K186" s="5">
         <v>0.4</v>
       </c>
-      <c r="L186" t="s">
+      <c r="N186" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A187" s="6">
         <v>44594</v>
       </c>
@@ -6771,11 +6797,11 @@
       <c r="K187" s="5">
         <v>0.4</v>
       </c>
-      <c r="L187" t="s">
+      <c r="N187" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A188" s="6">
         <v>44595</v>
       </c>
@@ -6803,11 +6829,11 @@
       <c r="H188" s="5">
         <v>1</v>
       </c>
-      <c r="L188" s="5" t="s">
+      <c r="N188" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A189" s="6">
         <v>44595</v>
       </c>
@@ -6832,11 +6858,11 @@
       <c r="H189" s="5">
         <v>1</v>
       </c>
-      <c r="L189" s="5" t="s">
+      <c r="N189" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A190" s="6">
         <v>44595</v>
       </c>
@@ -6861,11 +6887,11 @@
       <c r="H190" s="5">
         <v>1</v>
       </c>
-      <c r="L190" s="5" t="s">
+      <c r="N190" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A191" s="6">
         <v>44595</v>
       </c>
@@ -6899,11 +6925,11 @@
       <c r="K191" s="5">
         <v>0.4</v>
       </c>
-      <c r="L191" s="5" t="s">
+      <c r="N191" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A192" s="6">
         <v>44595</v>
       </c>
@@ -6937,11 +6963,11 @@
       <c r="K192" s="5">
         <v>0.4</v>
       </c>
-      <c r="L192" s="5" t="s">
+      <c r="N192" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A193" s="6">
         <v>44595</v>
       </c>
@@ -6975,11 +7001,11 @@
       <c r="K193" s="5">
         <v>0.4</v>
       </c>
-      <c r="L193" t="s">
+      <c r="N193" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A194" s="6">
         <v>44595</v>
       </c>
@@ -7011,13 +7037,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="K194" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="L194" t="s">
+        <v>1.75</v>
+      </c>
+      <c r="N194" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A195" s="6">
         <v>44595</v>
       </c>
@@ -7051,11 +7077,11 @@
       <c r="K195" s="5">
         <v>0.4</v>
       </c>
-      <c r="L195" s="5" t="s">
+      <c r="N195" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A196" s="6">
         <v>44595</v>
       </c>
@@ -7089,11 +7115,11 @@
       <c r="K196" s="5">
         <v>0.4</v>
       </c>
-      <c r="L196" s="5" t="s">
+      <c r="N196" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A197" s="6">
         <v>44595</v>
       </c>
@@ -7127,11 +7153,11 @@
       <c r="K197" s="5">
         <v>0.4</v>
       </c>
-      <c r="L197" s="5" t="s">
+      <c r="N197" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A198" s="6">
         <v>44595</v>
       </c>
@@ -7165,11 +7191,11 @@
       <c r="K198" s="5">
         <v>0.4</v>
       </c>
-      <c r="L198" s="5" t="s">
+      <c r="N198" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A199" s="6">
         <v>44595</v>
       </c>
@@ -7203,11 +7229,11 @@
       <c r="K199">
         <v>0.4</v>
       </c>
-      <c r="L199" s="5" t="s">
+      <c r="N199" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A200" s="6">
         <v>44595</v>
       </c>
@@ -7241,11 +7267,11 @@
       <c r="K200" s="5">
         <v>0.4</v>
       </c>
-      <c r="L200" s="5" t="s">
+      <c r="N200" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44652</v>
       </c>
@@ -7279,11 +7305,11 @@
       <c r="K201">
         <v>0.4</v>
       </c>
-      <c r="L201" t="s">
+      <c r="N201" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A202" s="6">
         <v>44652</v>
       </c>
@@ -7317,11 +7343,11 @@
       <c r="K202" s="5">
         <v>0.4</v>
       </c>
-      <c r="L202" s="5" t="s">
+      <c r="N202" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A203" s="6">
         <v>44652</v>
       </c>
@@ -7355,11 +7381,11 @@
       <c r="K203" s="5">
         <v>0.4</v>
       </c>
-      <c r="L203" s="5" t="s">
+      <c r="N203" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A204" s="6">
         <v>44652</v>
       </c>
@@ -7393,11 +7419,11 @@
       <c r="K204" s="5">
         <v>0.4</v>
       </c>
-      <c r="L204" s="5" t="s">
+      <c r="N204" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A205" s="6">
         <v>44652</v>
       </c>
@@ -7434,11 +7460,11 @@
       <c r="K205" s="5">
         <v>0.4</v>
       </c>
-      <c r="L205" t="s">
+      <c r="N205" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A206" s="6">
         <v>44652</v>
       </c>
@@ -7472,11 +7498,11 @@
       <c r="K206" s="5">
         <v>0.4</v>
       </c>
-      <c r="L206" s="5" t="s">
+      <c r="N206" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A207" s="6">
         <v>44652</v>
       </c>
@@ -7510,11 +7536,11 @@
       <c r="K207" s="5">
         <v>0.4</v>
       </c>
-      <c r="L207" s="5" t="s">
+      <c r="N207" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A208" s="6">
         <v>44652</v>
       </c>
@@ -7548,11 +7574,11 @@
       <c r="K208" s="5">
         <v>0.4</v>
       </c>
-      <c r="L208" s="5" t="s">
+      <c r="N208" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A209" s="6">
         <v>44652</v>
       </c>
@@ -7586,11 +7612,11 @@
       <c r="K209" s="5">
         <v>0.4</v>
       </c>
-      <c r="L209" s="5" t="s">
+      <c r="N209" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A210" s="6">
         <v>44652</v>
       </c>
@@ -7627,11 +7653,11 @@
       <c r="K210" s="5">
         <v>0.4</v>
       </c>
-      <c r="L210" s="5" t="s">
+      <c r="N210" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A211" s="6">
         <v>44652</v>
       </c>
@@ -7668,11 +7694,11 @@
       <c r="K211" s="5">
         <v>0.4</v>
       </c>
-      <c r="L211" s="5" t="s">
+      <c r="N211" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A212" s="6">
         <v>44652</v>
       </c>
@@ -7706,11 +7732,11 @@
       <c r="K212" s="5">
         <v>0.4</v>
       </c>
-      <c r="L212" s="5" t="s">
+      <c r="N212" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A213" s="6">
         <v>44652</v>
       </c>
@@ -7744,11 +7770,11 @@
       <c r="K213" s="5">
         <v>0.4</v>
       </c>
-      <c r="L213" s="5" t="s">
+      <c r="N213" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A214" s="6">
         <v>44652</v>
       </c>
@@ -7782,11 +7808,11 @@
       <c r="K214" s="5">
         <v>0.4</v>
       </c>
-      <c r="L214" s="5" t="s">
+      <c r="N214" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A215" s="6">
         <v>44652</v>
       </c>
@@ -7820,11 +7846,11 @@
       <c r="K215" s="5">
         <v>0.4</v>
       </c>
-      <c r="L215" s="5" t="s">
+      <c r="N215" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A216" s="6">
         <v>44652</v>
       </c>
@@ -7858,11 +7884,11 @@
       <c r="K216" s="5">
         <v>0.4</v>
       </c>
-      <c r="L216" s="5" t="s">
+      <c r="N216" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A217" s="6">
         <v>44652</v>
       </c>
@@ -7899,11 +7925,11 @@
       <c r="K217" s="5">
         <v>0.4</v>
       </c>
-      <c r="L217" s="5" t="s">
+      <c r="N217" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A218" s="6">
         <v>44652</v>
       </c>
@@ -7937,11 +7963,11 @@
       <c r="K218" s="5">
         <v>0.4</v>
       </c>
-      <c r="L218" s="5" t="s">
+      <c r="N218" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A219" s="6">
         <v>44652</v>
       </c>
@@ -7978,11 +8004,11 @@
       <c r="K219" s="5">
         <v>0.4</v>
       </c>
-      <c r="L219" s="5" t="s">
+      <c r="N219" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A220" s="6">
         <v>44652</v>
       </c>
@@ -8016,11 +8042,11 @@
       <c r="K220" s="5">
         <v>0.4</v>
       </c>
-      <c r="L220" s="5" t="s">
+      <c r="N220" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A221" s="6">
         <v>44652</v>
       </c>
@@ -8054,11 +8080,11 @@
       <c r="K221" s="5">
         <v>0.4</v>
       </c>
-      <c r="L221" s="5" t="s">
+      <c r="N221" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A222" s="6">
         <v>44652</v>
       </c>
@@ -8092,11 +8118,11 @@
       <c r="K222" s="5">
         <v>0.4</v>
       </c>
-      <c r="L222" s="5" t="s">
+      <c r="N222" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A223" s="6">
         <v>44652</v>
       </c>
@@ -8130,11 +8156,11 @@
       <c r="K223" s="5">
         <v>0.4</v>
       </c>
-      <c r="L223" s="5" t="s">
+      <c r="N223" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A224" s="6">
         <v>44652</v>
       </c>
@@ -8168,11 +8194,11 @@
       <c r="K224" s="5">
         <v>0.4</v>
       </c>
-      <c r="L224" s="5" t="s">
+      <c r="N224" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>44658</v>
       </c>
@@ -8206,11 +8232,11 @@
       <c r="K225">
         <v>0.4</v>
       </c>
-      <c r="L225" t="s">
+      <c r="N225" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>44658</v>
       </c>
@@ -8244,11 +8270,11 @@
       <c r="K226">
         <v>0.4</v>
       </c>
-      <c r="L226" t="s">
+      <c r="N226" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>44658</v>
       </c>
@@ -8282,11 +8308,11 @@
       <c r="K227">
         <v>0.4</v>
       </c>
-      <c r="L227" t="s">
+      <c r="N227" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>44658</v>
       </c>
@@ -8320,11 +8346,11 @@
       <c r="K228">
         <v>0.4</v>
       </c>
-      <c r="L228" t="s">
+      <c r="N228" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>44658</v>
       </c>
@@ -8358,11 +8384,11 @@
       <c r="K229">
         <v>0.4</v>
       </c>
-      <c r="L229" t="s">
+      <c r="N229" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>44658</v>
       </c>
@@ -8396,11 +8422,11 @@
       <c r="K230">
         <v>0.4</v>
       </c>
-      <c r="L230" t="s">
+      <c r="N230" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>44658</v>
       </c>
@@ -8434,11 +8460,11 @@
       <c r="K231">
         <v>0.4</v>
       </c>
-      <c r="L231" t="s">
+      <c r="N231" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>44658</v>
       </c>
@@ -8472,11 +8498,11 @@
       <c r="K232">
         <v>0.4</v>
       </c>
-      <c r="L232" t="s">
+      <c r="N232" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>44658</v>
       </c>
@@ -8510,11 +8536,11 @@
       <c r="K233">
         <v>0.4</v>
       </c>
-      <c r="L233" t="s">
+      <c r="N233" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>44659</v>
       </c>
@@ -8548,11 +8574,11 @@
       <c r="K234">
         <v>0.4</v>
       </c>
-      <c r="L234" t="s">
+      <c r="N234" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>44659</v>
       </c>
@@ -8586,11 +8612,11 @@
       <c r="K235">
         <v>0.4</v>
       </c>
-      <c r="L235" t="s">
+      <c r="N235" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>44659</v>
       </c>
@@ -8624,11 +8650,11 @@
       <c r="K236">
         <v>0.4</v>
       </c>
-      <c r="L236" t="s">
+      <c r="N236" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>44659</v>
       </c>
@@ -8662,11 +8688,11 @@
       <c r="K237">
         <v>0.4</v>
       </c>
-      <c r="L237" t="s">
+      <c r="N237" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>44659</v>
       </c>
@@ -8700,11 +8726,11 @@
       <c r="K238">
         <v>0.4</v>
       </c>
-      <c r="L238" t="s">
+      <c r="N238" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>44659</v>
       </c>
@@ -8738,11 +8764,11 @@
       <c r="K239">
         <v>0.4</v>
       </c>
-      <c r="L239" t="s">
+      <c r="N239" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>44818</v>
       </c>
@@ -8776,11 +8802,11 @@
       <c r="K240">
         <v>1</v>
       </c>
-      <c r="L240" t="s">
+      <c r="N240" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>44818</v>
       </c>
@@ -8814,11 +8840,11 @@
       <c r="K241">
         <v>1</v>
       </c>
-      <c r="L241" t="s">
+      <c r="N241" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>44818</v>
       </c>
@@ -8852,11 +8878,11 @@
       <c r="K242">
         <v>1</v>
       </c>
-      <c r="L242" t="s">
+      <c r="N242" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>44818</v>
       </c>
@@ -8890,11 +8916,11 @@
       <c r="K243">
         <v>1</v>
       </c>
-      <c r="L243" t="s">
+      <c r="N243" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>44818</v>
       </c>
@@ -8908,31 +8934,31 @@
         <v>5</v>
       </c>
       <c r="E244">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F244">
-        <v>3.5000000000000003E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G244">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="H244">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I244">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="J244">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K244">
         <v>1</v>
       </c>
-      <c r="L244" t="s">
+      <c r="N244" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>44818</v>
       </c>
@@ -8946,31 +8972,31 @@
         <v>5</v>
       </c>
       <c r="E245">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F245">
-        <v>3.5000000000000003E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G245">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="H245">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I245">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="J245">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K245">
         <v>1</v>
       </c>
-      <c r="L245" t="s">
+      <c r="N245" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>44823</v>
       </c>
@@ -9004,11 +9030,11 @@
       <c r="K246">
         <v>1</v>
       </c>
-      <c r="L246" t="s">
+      <c r="N246" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>44823</v>
       </c>
@@ -9042,11 +9068,11 @@
       <c r="K247">
         <v>1</v>
       </c>
-      <c r="L247" t="s">
+      <c r="N247" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>44823</v>
       </c>
@@ -9080,11 +9106,11 @@
       <c r="K248">
         <v>1</v>
       </c>
-      <c r="L248" t="s">
+      <c r="N248" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>44823</v>
       </c>
@@ -9118,11 +9144,11 @@
       <c r="K249">
         <v>1</v>
       </c>
-      <c r="L249" t="s">
+      <c r="N249" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>44824</v>
       </c>
@@ -9156,11 +9182,11 @@
       <c r="K250">
         <v>1</v>
       </c>
-      <c r="L250" t="s">
+      <c r="N250" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>44824</v>
       </c>
@@ -9194,11 +9220,11 @@
       <c r="K251">
         <v>1</v>
       </c>
-      <c r="L251" t="s">
+      <c r="N251" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>44824</v>
       </c>
@@ -9232,11 +9258,11 @@
       <c r="K252">
         <v>1</v>
       </c>
-      <c r="L252" t="s">
+      <c r="N252" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>44824</v>
       </c>
@@ -9270,11 +9296,11 @@
       <c r="K253">
         <v>1</v>
       </c>
-      <c r="L253" t="s">
+      <c r="N253" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>44824</v>
       </c>
@@ -9308,11 +9334,11 @@
       <c r="K254">
         <v>1</v>
       </c>
-      <c r="L254" t="s">
+      <c r="N254" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>44824</v>
       </c>
@@ -9346,11 +9372,11 @@
       <c r="K255">
         <v>1</v>
       </c>
-      <c r="L255" t="s">
+      <c r="N255" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>44824</v>
       </c>
@@ -9384,11 +9410,11 @@
       <c r="K256">
         <v>1</v>
       </c>
-      <c r="L256" t="s">
+      <c r="N256" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>44824</v>
       </c>
@@ -9422,8 +9448,754 @@
       <c r="K257">
         <v>1</v>
       </c>
-      <c r="L257" t="s">
+      <c r="N257" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="258" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A258" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B258">
+        <v>37</v>
+      </c>
+      <c r="C258">
+        <v>9</v>
+      </c>
+      <c r="D258" t="s">
+        <v>5</v>
+      </c>
+      <c r="E258">
+        <v>0.02</v>
+      </c>
+      <c r="F258">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G258">
+        <v>6.25</v>
+      </c>
+      <c r="H258">
+        <v>0</v>
+      </c>
+      <c r="I258">
+        <v>0</v>
+      </c>
+      <c r="J258">
+        <v>1</v>
+      </c>
+      <c r="K258">
+        <v>1</v>
+      </c>
+      <c r="N258" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="259" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A259" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B259">
+        <v>37</v>
+      </c>
+      <c r="C259">
+        <v>10</v>
+      </c>
+      <c r="D259" t="s">
+        <v>5</v>
+      </c>
+      <c r="E259">
+        <v>0.02</v>
+      </c>
+      <c r="F259">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G259">
+        <v>6.25</v>
+      </c>
+      <c r="H259">
+        <v>0</v>
+      </c>
+      <c r="I259">
+        <v>0</v>
+      </c>
+      <c r="J259">
+        <v>1</v>
+      </c>
+      <c r="K259">
+        <v>1</v>
+      </c>
+      <c r="N259" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="260" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A260" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B260">
+        <v>37</v>
+      </c>
+      <c r="C260">
+        <v>27</v>
+      </c>
+      <c r="D260" t="s">
+        <v>5</v>
+      </c>
+      <c r="E260">
+        <v>0.1</v>
+      </c>
+      <c r="F260">
+        <v>0.7</v>
+      </c>
+      <c r="G260">
+        <v>1.25</v>
+      </c>
+      <c r="H260">
+        <v>0</v>
+      </c>
+      <c r="I260">
+        <v>0</v>
+      </c>
+      <c r="J260">
+        <v>0.4</v>
+      </c>
+      <c r="K260">
+        <v>1.5</v>
+      </c>
+      <c r="N260" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="261" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A261" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B261">
+        <v>37</v>
+      </c>
+      <c r="C261">
+        <v>28</v>
+      </c>
+      <c r="D261" t="s">
+        <v>5</v>
+      </c>
+      <c r="E261">
+        <v>0.01</v>
+      </c>
+      <c r="F261">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G261">
+        <v>12.5</v>
+      </c>
+      <c r="H261">
+        <v>0</v>
+      </c>
+      <c r="I261">
+        <v>0</v>
+      </c>
+      <c r="J261">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K261">
+        <v>1</v>
+      </c>
+      <c r="N261" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="262" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A262" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B262">
+        <v>37</v>
+      </c>
+      <c r="C262">
+        <v>29</v>
+      </c>
+      <c r="D262" t="s">
+        <v>5</v>
+      </c>
+      <c r="E262">
+        <v>0.01</v>
+      </c>
+      <c r="F262">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G262">
+        <v>12.5</v>
+      </c>
+      <c r="H262">
+        <v>0</v>
+      </c>
+      <c r="I262">
+        <v>0</v>
+      </c>
+      <c r="J262">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K262">
+        <v>1</v>
+      </c>
+      <c r="N262" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="263" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A263" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B263">
+        <v>37</v>
+      </c>
+      <c r="C263">
+        <v>30</v>
+      </c>
+      <c r="D263" t="s">
+        <v>5</v>
+      </c>
+      <c r="E263">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F263">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G263">
+        <v>25</v>
+      </c>
+      <c r="H263">
+        <v>0</v>
+      </c>
+      <c r="I263">
+        <v>0</v>
+      </c>
+      <c r="J263">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K263">
+        <v>1</v>
+      </c>
+      <c r="N263" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="264" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A264" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B264">
+        <v>37</v>
+      </c>
+      <c r="C264">
+        <v>31</v>
+      </c>
+      <c r="D264" t="s">
+        <v>5</v>
+      </c>
+      <c r="E264">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F264">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G264">
+        <v>25</v>
+      </c>
+      <c r="H264">
+        <v>0</v>
+      </c>
+      <c r="I264">
+        <v>0</v>
+      </c>
+      <c r="J264">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K264">
+        <v>1</v>
+      </c>
+      <c r="N264" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="265" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A265" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B265">
+        <v>38</v>
+      </c>
+      <c r="C265">
+        <v>41</v>
+      </c>
+      <c r="D265" t="s">
+        <v>5</v>
+      </c>
+      <c r="E265">
+        <v>0.02</v>
+      </c>
+      <c r="F265">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G265">
+        <v>6.25</v>
+      </c>
+      <c r="H265">
+        <v>0</v>
+      </c>
+      <c r="I265">
+        <v>0</v>
+      </c>
+      <c r="J265">
+        <v>1</v>
+      </c>
+      <c r="K265">
+        <v>1</v>
+      </c>
+      <c r="N265" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="266" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A266" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B266">
+        <v>38</v>
+      </c>
+      <c r="C266">
+        <v>42</v>
+      </c>
+      <c r="D266" t="s">
+        <v>5</v>
+      </c>
+      <c r="E266">
+        <v>0.02</v>
+      </c>
+      <c r="F266">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G266">
+        <v>6.25</v>
+      </c>
+      <c r="H266">
+        <v>0</v>
+      </c>
+      <c r="I266">
+        <v>0</v>
+      </c>
+      <c r="J266">
+        <v>1</v>
+      </c>
+      <c r="K266">
+        <v>1</v>
+      </c>
+      <c r="N266" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="267" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A267" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B267">
+        <v>38</v>
+      </c>
+      <c r="C267">
+        <v>51</v>
+      </c>
+      <c r="D267" t="s">
+        <v>5</v>
+      </c>
+      <c r="E267">
+        <v>0.01</v>
+      </c>
+      <c r="F267">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G267">
+        <v>12.5</v>
+      </c>
+      <c r="H267">
+        <v>0</v>
+      </c>
+      <c r="I267">
+        <v>0</v>
+      </c>
+      <c r="J267">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K267">
+        <v>1</v>
+      </c>
+      <c r="N267" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="268" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A268" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B268">
+        <v>38</v>
+      </c>
+      <c r="C268">
+        <v>52</v>
+      </c>
+      <c r="D268" t="s">
+        <v>5</v>
+      </c>
+      <c r="E268">
+        <v>0.01</v>
+      </c>
+      <c r="F268">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G268">
+        <v>12.5</v>
+      </c>
+      <c r="H268">
+        <v>0</v>
+      </c>
+      <c r="I268">
+        <v>-1</v>
+      </c>
+      <c r="J268">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K268">
+        <v>1.4</v>
+      </c>
+      <c r="N268" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="269" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A269" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B269">
+        <v>38</v>
+      </c>
+      <c r="C269">
+        <v>61</v>
+      </c>
+      <c r="D269" t="s">
+        <v>5</v>
+      </c>
+      <c r="E269">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F269">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G269">
+        <v>25</v>
+      </c>
+      <c r="H269">
+        <v>0</v>
+      </c>
+      <c r="I269">
+        <v>0</v>
+      </c>
+      <c r="J269">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K269">
+        <v>1</v>
+      </c>
+      <c r="N269" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="270" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A270" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B270">
+        <v>38</v>
+      </c>
+      <c r="C270">
+        <v>62</v>
+      </c>
+      <c r="D270" t="s">
+        <v>5</v>
+      </c>
+      <c r="E270">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F270">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G270">
+        <v>25</v>
+      </c>
+      <c r="H270">
+        <v>0</v>
+      </c>
+      <c r="I270">
+        <v>0</v>
+      </c>
+      <c r="J270">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K270">
+        <v>1</v>
+      </c>
+      <c r="N270" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="271" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A271" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B271">
+        <v>38</v>
+      </c>
+      <c r="C271">
+        <v>63</v>
+      </c>
+      <c r="D271" t="s">
+        <v>5</v>
+      </c>
+      <c r="E271">
+        <v>0.01</v>
+      </c>
+      <c r="F271">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G271">
+        <v>12.5</v>
+      </c>
+      <c r="H271">
+        <v>0</v>
+      </c>
+      <c r="I271">
+        <v>-0.5</v>
+      </c>
+      <c r="J271">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K271">
+        <v>1.4</v>
+      </c>
+      <c r="N271" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="272" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A272" s="1">
+        <v>44839</v>
+      </c>
+      <c r="B272">
+        <v>38</v>
+      </c>
+      <c r="C272">
+        <v>64</v>
+      </c>
+      <c r="D272" t="s">
+        <v>5</v>
+      </c>
+      <c r="E272">
+        <v>0.01</v>
+      </c>
+      <c r="F272">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G272">
+        <v>12.5</v>
+      </c>
+      <c r="H272">
+        <v>0</v>
+      </c>
+      <c r="I272">
+        <v>-1</v>
+      </c>
+      <c r="J272">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K272">
+        <v>1.4</v>
+      </c>
+      <c r="N272" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="273" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A273" s="6">
+        <v>44839</v>
+      </c>
+      <c r="B273">
+        <v>38</v>
+      </c>
+      <c r="C273">
+        <v>65</v>
+      </c>
+      <c r="D273" t="s">
+        <v>5</v>
+      </c>
+      <c r="E273" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F273" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G273" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="H273" s="5">
+        <v>0</v>
+      </c>
+      <c r="I273" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="J273" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K273" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="L273">
+        <v>1</v>
+      </c>
+      <c r="M273">
+        <v>5</v>
+      </c>
+      <c r="N273" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="274" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A274" s="6">
+        <v>44839</v>
+      </c>
+      <c r="B274">
+        <v>38</v>
+      </c>
+      <c r="C274">
+        <v>66</v>
+      </c>
+      <c r="D274" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E274" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F274" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G274" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="H274" s="5">
+        <v>0</v>
+      </c>
+      <c r="I274" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="J274" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K274" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="L274">
+        <v>1</v>
+      </c>
+      <c r="M274">
+        <v>10</v>
+      </c>
+      <c r="N274" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="275" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A275" s="6">
+        <v>44839</v>
+      </c>
+      <c r="B275">
+        <v>38</v>
+      </c>
+      <c r="C275">
+        <v>67</v>
+      </c>
+      <c r="D275" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E275" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F275" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G275" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="H275" s="5">
+        <v>0</v>
+      </c>
+      <c r="I275" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="J275" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K275" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="L275">
+        <v>1</v>
+      </c>
+      <c r="M275">
+        <v>10</v>
+      </c>
+      <c r="N275" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="276" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A276" s="6">
+        <v>44839</v>
+      </c>
+      <c r="B276">
+        <v>38</v>
+      </c>
+      <c r="C276">
+        <v>68</v>
+      </c>
+      <c r="D276" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E276" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F276" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G276" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="H276" s="5">
+        <v>0</v>
+      </c>
+      <c r="I276" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="J276" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K276" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="L276">
+        <v>1</v>
+      </c>
+      <c r="M276">
+        <v>5</v>
+      </c>
+      <c r="N276" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes to time frequency
</commit_message>
<xml_diff>
--- a/fly_record.xlsx
+++ b/fly_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\group_swinderen\Dinis\Sequential Effects ERP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39E3C8E-7351-4330-94AA-491E358B2D68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0168D1E-9AD0-48C9-A1FD-BA1D3DB436E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10800" windowHeight="5190" xr2:uid="{0C11348E-E482-4597-B3FE-1374AFB87193}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="109">
   <si>
     <t>Date</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Bruno: Looks bad; Dinis: it is fine</t>
-  </si>
-  <si>
-    <t>Bruno: A bit iffy; Dinis: it's fine</t>
   </si>
   <si>
     <t>Crashed around 50 mins</t>
@@ -286,6 +283,114 @@
   <si>
     <t>LFPChannel</t>
   </si>
+  <si>
+    <t>regular, front, no ATR; DINIS: data very iffy even after filtering</t>
+  </si>
+  <si>
+    <r>
+      <t>regular, front, no ATR;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> PHOT jitttery</t>
+    </r>
+  </si>
+  <si>
+    <t>Awful PHOT jitttering, no v-sync</t>
+  </si>
+  <si>
+    <t>regular,sides, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular,adjfront, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular,adjleft, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular,adjright, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular,checkfront4, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular,checkfront6, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular,checkfront2, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular,checkfront3, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular,checkfront1, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular,checkfront5, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular,checkleft4, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular,checkright4, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular,checkfront,no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular,adjfront,no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular,sides,no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular, adjfront, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular, adjleft, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular, adjright, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular, checkfront4, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular, checkleft4, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular, checkright4, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular, checkfront1, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular, checkfront2, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular, checkfront3, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular, checkfront5, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular, checkfront6, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular, checkleft2, no ATR, blue</t>
+  </si>
+  <si>
+    <t>regular, checkright2, no ATR, blue</t>
+  </si>
+  <si>
+    <t>Frozen?, adjfront, no ATR, blue</t>
+  </si>
 </sst>
 </file>
 
@@ -294,7 +399,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/mm/yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,6 +418,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -338,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -347,6 +466,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680E0717-9BF1-4D4C-A430-96F9A20E59A5}">
-  <dimension ref="A1:P309"/>
+  <dimension ref="A1:P346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F262" workbookViewId="0">
-      <selection activeCell="O283" sqref="O283"/>
+    <sheetView tabSelected="1" topLeftCell="F297" workbookViewId="0">
+      <selection activeCell="N306" sqref="N306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,25 +826,25 @@
         <v>19</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="N1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>7</v>
@@ -764,6 +884,12 @@
       <c r="K2">
         <v>0.4</v>
       </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -790,6 +916,12 @@
       <c r="H3">
         <v>0</v>
       </c>
+      <c r="N3" s="5">
+        <v>2</v>
+      </c>
+      <c r="O3" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -825,6 +957,15 @@
       <c r="K4">
         <v>0.4</v>
       </c>
+      <c r="N4" s="5">
+        <v>2</v>
+      </c>
+      <c r="O4" s="5">
+        <v>1</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -851,6 +992,12 @@
       <c r="H5">
         <v>0</v>
       </c>
+      <c r="N5" s="5">
+        <v>2</v>
+      </c>
+      <c r="O5" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -886,6 +1033,15 @@
       <c r="K6" s="5">
         <v>0.2</v>
       </c>
+      <c r="N6" s="5">
+        <v>2</v>
+      </c>
+      <c r="O6" s="5">
+        <v>1</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -912,6 +1068,12 @@
       <c r="H7">
         <v>0</v>
       </c>
+      <c r="N7" s="5">
+        <v>2</v>
+      </c>
+      <c r="O7" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -947,6 +1109,15 @@
       <c r="K8" s="5">
         <v>0.2</v>
       </c>
+      <c r="N8" s="5">
+        <v>2</v>
+      </c>
+      <c r="O8" s="5">
+        <v>1</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -982,6 +1153,15 @@
       <c r="K9" s="5">
         <v>0.2</v>
       </c>
+      <c r="N9" s="5">
+        <v>2</v>
+      </c>
+      <c r="O9" s="5">
+        <v>1</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1008,6 +1188,12 @@
       <c r="H10">
         <v>0</v>
       </c>
+      <c r="N10" s="5">
+        <v>2</v>
+      </c>
+      <c r="O10" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1043,6 +1229,12 @@
       <c r="K11" s="5">
         <v>0.4</v>
       </c>
+      <c r="N11" s="5">
+        <v>2</v>
+      </c>
+      <c r="O11" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1069,6 +1261,12 @@
       <c r="H12">
         <v>0</v>
       </c>
+      <c r="N12" s="5">
+        <v>2</v>
+      </c>
+      <c r="O12" s="5">
+        <v>1</v>
+      </c>
       <c r="P12" t="s">
         <v>17</v>
       </c>
@@ -1107,6 +1305,15 @@
       <c r="K13" s="5">
         <v>0.4</v>
       </c>
+      <c r="N13" s="5">
+        <v>2</v>
+      </c>
+      <c r="O13" s="5">
+        <v>1</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1133,6 +1340,12 @@
       <c r="H14">
         <v>0</v>
       </c>
+      <c r="N14" s="5">
+        <v>2</v>
+      </c>
+      <c r="O14" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -1168,6 +1381,12 @@
       <c r="K15" s="5">
         <v>0.4</v>
       </c>
+      <c r="N15" s="5">
+        <v>2</v>
+      </c>
+      <c r="O15" s="5">
+        <v>1</v>
+      </c>
       <c r="P15" t="s">
         <v>21</v>
       </c>
@@ -1201,13 +1420,19 @@
         <v>0</v>
       </c>
       <c r="J16" s="5">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K16" s="5">
         <v>0.4</v>
       </c>
-      <c r="P16" t="s">
-        <v>22</v>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1235,6 +1460,12 @@
       <c r="H17" s="4">
         <v>1</v>
       </c>
+      <c r="N17" s="5">
+        <v>2</v>
+      </c>
+      <c r="O17" s="5">
+        <v>1</v>
+      </c>
       <c r="P17" t="s">
         <v>20</v>
       </c>
@@ -1273,6 +1504,15 @@
       <c r="K18" s="5">
         <v>0.4</v>
       </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18" s="8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -1299,6 +1539,12 @@
       <c r="H19" s="4">
         <v>0</v>
       </c>
+      <c r="N19" s="5">
+        <v>2</v>
+      </c>
+      <c r="O19" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -1334,6 +1580,12 @@
       <c r="K20" s="5">
         <v>0.4</v>
       </c>
+      <c r="N20">
+        <v>2</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -1369,6 +1621,12 @@
       <c r="K21" s="5">
         <v>0.4</v>
       </c>
+      <c r="N21">
+        <v>2</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -1395,8 +1653,14 @@
       <c r="H22" s="4">
         <v>0</v>
       </c>
+      <c r="N22" s="5">
+        <v>2</v>
+      </c>
+      <c r="O22" s="5">
+        <v>1</v>
+      </c>
       <c r="P22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -1424,6 +1688,12 @@
       <c r="H23" s="4">
         <v>0</v>
       </c>
+      <c r="N23" s="5">
+        <v>2</v>
+      </c>
+      <c r="O23" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -1459,6 +1729,12 @@
       <c r="K24" s="5">
         <v>0.4</v>
       </c>
+      <c r="N24">
+        <v>2</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -1488,6 +1764,12 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
+      <c r="N25" s="5">
+        <v>2</v>
+      </c>
+      <c r="O25" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -1514,6 +1796,12 @@
       <c r="H26" s="4">
         <v>0</v>
       </c>
+      <c r="N26" s="5">
+        <v>2</v>
+      </c>
+      <c r="O26" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
@@ -1549,6 +1837,12 @@
       <c r="K27" s="5">
         <v>0.4</v>
       </c>
+      <c r="N27">
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -1575,6 +1869,12 @@
       <c r="H28" s="4">
         <v>0</v>
       </c>
+      <c r="N28" s="5">
+        <v>2</v>
+      </c>
+      <c r="O28" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -1610,6 +1910,12 @@
       <c r="K29" s="5">
         <v>0.4</v>
       </c>
+      <c r="N29">
+        <v>2</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -1636,6 +1942,12 @@
       <c r="H30" s="4">
         <v>0</v>
       </c>
+      <c r="N30" s="5">
+        <v>2</v>
+      </c>
+      <c r="O30" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -1678,7 +1990,7 @@
         <v>1</v>
       </c>
       <c r="P31" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -1706,6 +2018,12 @@
       <c r="H32" s="4">
         <v>0</v>
       </c>
+      <c r="N32" s="5">
+        <v>2</v>
+      </c>
+      <c r="O32" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
@@ -1741,6 +2059,12 @@
       <c r="K33" s="5">
         <v>0.4</v>
       </c>
+      <c r="N33">
+        <v>2</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
@@ -2989,7 +3313,7 @@
         <v>1</v>
       </c>
       <c r="P74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -3058,6 +3382,12 @@
       <c r="K76" s="5">
         <v>0.4</v>
       </c>
+      <c r="N76">
+        <v>2</v>
+      </c>
+      <c r="O76">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
@@ -3513,7 +3843,7 @@
         <v>0.4</v>
       </c>
       <c r="P90" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
@@ -3918,7 +4248,7 @@
         <v>1</v>
       </c>
       <c r="P102" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
@@ -3950,7 +4280,7 @@
         <v>0</v>
       </c>
       <c r="P103" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
@@ -3997,7 +4327,7 @@
         <v>1</v>
       </c>
       <c r="P104" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
@@ -4029,7 +4359,7 @@
         <v>0</v>
       </c>
       <c r="P105" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
@@ -4070,7 +4400,7 @@
         <v>0.4</v>
       </c>
       <c r="P106" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
@@ -4102,7 +4432,7 @@
         <v>0</v>
       </c>
       <c r="P107" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
@@ -4134,7 +4464,7 @@
         <v>0</v>
       </c>
       <c r="P108" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
@@ -4166,7 +4496,7 @@
         <v>0</v>
       </c>
       <c r="P109" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
@@ -4198,7 +4528,7 @@
         <v>0</v>
       </c>
       <c r="P110" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
@@ -4230,7 +4560,7 @@
         <v>0</v>
       </c>
       <c r="P111" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
@@ -4270,8 +4600,14 @@
       <c r="K112" s="5">
         <v>0.4</v>
       </c>
+      <c r="N112">
+        <v>2</v>
+      </c>
+      <c r="O112">
+        <v>1</v>
+      </c>
       <c r="P112" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
@@ -4303,7 +4639,7 @@
         <v>0</v>
       </c>
       <c r="P113" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
@@ -4343,8 +4679,14 @@
       <c r="K114" s="5">
         <v>0.4</v>
       </c>
+      <c r="N114">
+        <v>2</v>
+      </c>
+      <c r="O114">
+        <v>1</v>
+      </c>
       <c r="P114" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
@@ -4740,7 +5082,7 @@
         <v>0.4</v>
       </c>
       <c r="P126" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
@@ -4769,7 +5111,7 @@
         <v>0</v>
       </c>
       <c r="P127" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
@@ -4815,7 +5157,7 @@
         <v>1</v>
       </c>
       <c r="P128" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.25">
@@ -4846,7 +5188,7 @@
         <v>0</v>
       </c>
       <c r="P129" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.25">
@@ -4884,7 +5226,7 @@
         <v>0.4</v>
       </c>
       <c r="P130" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.25">
@@ -4913,7 +5255,7 @@
         <v>0</v>
       </c>
       <c r="P131" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.25">
@@ -4953,7 +5295,7 @@
         <v>0.4</v>
       </c>
       <c r="P132" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.25">
@@ -4991,7 +5333,7 @@
         <v>0.4</v>
       </c>
       <c r="P133" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
@@ -5020,7 +5362,7 @@
         <v>0</v>
       </c>
       <c r="P134" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
@@ -5066,7 +5408,7 @@
         <v>1</v>
       </c>
       <c r="P135" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.25">
@@ -5097,7 +5439,7 @@
         <v>0</v>
       </c>
       <c r="P136" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.25">
@@ -5135,7 +5477,7 @@
         <v>0.1</v>
       </c>
       <c r="P137" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.25">
@@ -5164,7 +5506,7 @@
         <v>0</v>
       </c>
       <c r="P138" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.25">
@@ -5210,7 +5552,7 @@
         <v>1</v>
       </c>
       <c r="P139" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.25">
@@ -5241,7 +5583,7 @@
         <v>0</v>
       </c>
       <c r="P140" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.25">
@@ -5279,7 +5621,7 @@
         <v>0.1</v>
       </c>
       <c r="P141" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.25">
@@ -5308,7 +5650,7 @@
         <v>0</v>
       </c>
       <c r="P142" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.25">
@@ -5339,7 +5681,7 @@
         <v>0</v>
       </c>
       <c r="P143" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.25">
@@ -5379,7 +5721,7 @@
         <v>0.4</v>
       </c>
       <c r="P144" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.25">
@@ -5417,7 +5759,7 @@
         <v>0.1</v>
       </c>
       <c r="P145" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.25">
@@ -5446,7 +5788,7 @@
         <v>0</v>
       </c>
       <c r="P146" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.25">
@@ -5492,7 +5834,7 @@
         <v>1</v>
       </c>
       <c r="P147" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.25">
@@ -5523,7 +5865,7 @@
         <v>0</v>
       </c>
       <c r="P148" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.25">
@@ -5561,7 +5903,7 @@
         <v>0.1</v>
       </c>
       <c r="P149" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.25">
@@ -5590,7 +5932,7 @@
         <v>0</v>
       </c>
       <c r="P150" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.25">
@@ -5636,7 +5978,7 @@
         <v>1</v>
       </c>
       <c r="P151" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.25">
@@ -5667,7 +6009,7 @@
         <v>0</v>
       </c>
       <c r="P152" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
@@ -5705,7 +6047,7 @@
         <v>0.4</v>
       </c>
       <c r="P153" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.25">
@@ -5734,7 +6076,7 @@
         <v>0</v>
       </c>
       <c r="P154" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.25">
@@ -5772,7 +6114,7 @@
         <v>0.4</v>
       </c>
       <c r="P155" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.25">
@@ -5812,7 +6154,7 @@
         <v>0.4</v>
       </c>
       <c r="P156" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.25">
@@ -5843,7 +6185,7 @@
         <v>0</v>
       </c>
       <c r="P157" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.25">
@@ -5872,7 +6214,7 @@
         <v>0</v>
       </c>
       <c r="P158" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.25">
@@ -5910,7 +6252,7 @@
         <v>0.4</v>
       </c>
       <c r="P159" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.25">
@@ -5939,7 +6281,7 @@
         <v>0</v>
       </c>
       <c r="P160" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.25">
@@ -5970,7 +6312,7 @@
         <v>0</v>
       </c>
       <c r="P161" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.25">
@@ -6016,7 +6358,7 @@
         <v>1</v>
       </c>
       <c r="P162" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.25">
@@ -6054,7 +6396,7 @@
         <v>0.4</v>
       </c>
       <c r="P163" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.25">
@@ -6094,7 +6436,7 @@
         <v>0.1</v>
       </c>
       <c r="P164" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.25">
@@ -6134,7 +6476,7 @@
         <v>0.4</v>
       </c>
       <c r="P165" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.25">
@@ -6172,7 +6514,7 @@
         <v>0.4</v>
       </c>
       <c r="P166" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.25">
@@ -6210,7 +6552,7 @@
         <v>0.4</v>
       </c>
       <c r="P167" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.25">
@@ -6250,7 +6592,7 @@
         <v>0.1</v>
       </c>
       <c r="P168" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.25">
@@ -6290,7 +6632,7 @@
         <v>0.4</v>
       </c>
       <c r="P169" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.25">
@@ -6328,7 +6670,7 @@
         <v>0.4</v>
       </c>
       <c r="P170" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.25">
@@ -6368,7 +6710,7 @@
         <v>0.4</v>
       </c>
       <c r="P171" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.25">
@@ -6399,7 +6741,7 @@
         <v>0</v>
       </c>
       <c r="P172" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.25">
@@ -6437,7 +6779,7 @@
         <v>0.4</v>
       </c>
       <c r="P173" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.25">
@@ -6466,7 +6808,7 @@
         <v>0</v>
       </c>
       <c r="P174" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.25">
@@ -6504,7 +6846,7 @@
         <v>0.4</v>
       </c>
       <c r="P175" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.25">
@@ -6533,7 +6875,7 @@
         <v>0</v>
       </c>
       <c r="P176" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.25">
@@ -6571,7 +6913,7 @@
         <v>0.4</v>
       </c>
       <c r="P177" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.25">
@@ -6611,7 +6953,7 @@
         <v>0.4</v>
       </c>
       <c r="P178" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.25">
@@ -6649,7 +6991,7 @@
         <v>0.4</v>
       </c>
       <c r="P179" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.25">
@@ -6695,7 +7037,7 @@
         <v>1</v>
       </c>
       <c r="P180" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.25">
@@ -6724,7 +7066,7 @@
         <v>0</v>
       </c>
       <c r="P181" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.25">
@@ -6756,7 +7098,7 @@
         <v>0</v>
       </c>
       <c r="P182" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.25">
@@ -6796,8 +7138,14 @@
       <c r="K183" s="5">
         <v>0.4</v>
       </c>
+      <c r="N183">
+        <v>2</v>
+      </c>
+      <c r="O183">
+        <v>1</v>
+      </c>
       <c r="P183" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.25">
@@ -6835,7 +7183,7 @@
         <v>0.4</v>
       </c>
       <c r="P184" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.25">
@@ -6873,7 +7221,7 @@
         <v>0.4</v>
       </c>
       <c r="P185" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.25">
@@ -6911,7 +7259,7 @@
         <v>0.4</v>
       </c>
       <c r="P186" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.25">
@@ -6949,7 +7297,7 @@
         <v>0.4</v>
       </c>
       <c r="P187" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.25">
@@ -6981,7 +7329,7 @@
         <v>1</v>
       </c>
       <c r="P188" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.25">
@@ -7010,7 +7358,7 @@
         <v>1</v>
       </c>
       <c r="P189" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.25">
@@ -7039,7 +7387,7 @@
         <v>1</v>
       </c>
       <c r="P190" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.25">
@@ -7077,7 +7425,7 @@
         <v>0.4</v>
       </c>
       <c r="P191" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.25">
@@ -7121,7 +7469,7 @@
         <v>1</v>
       </c>
       <c r="P192" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.25">
@@ -7159,7 +7507,7 @@
         <v>0.4</v>
       </c>
       <c r="P193" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.25">
@@ -7196,8 +7544,14 @@
       <c r="K194" s="5">
         <v>1.75</v>
       </c>
+      <c r="N194">
+        <v>1</v>
+      </c>
+      <c r="O194">
+        <v>1</v>
+      </c>
       <c r="P194" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.25">
@@ -7235,7 +7589,7 @@
         <v>0.4</v>
       </c>
       <c r="P195" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="196" spans="1:16" x14ac:dyDescent="0.25">
@@ -7273,7 +7627,7 @@
         <v>0.4</v>
       </c>
       <c r="P196" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="197" spans="1:16" x14ac:dyDescent="0.25">
@@ -7317,7 +7671,7 @@
         <v>1</v>
       </c>
       <c r="P197" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="198" spans="1:16" x14ac:dyDescent="0.25">
@@ -7355,7 +7709,7 @@
         <v>0.4</v>
       </c>
       <c r="P198" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.25">
@@ -7393,7 +7747,7 @@
         <v>0.4</v>
       </c>
       <c r="P199" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="200" spans="1:16" x14ac:dyDescent="0.25">
@@ -7430,8 +7784,14 @@
       <c r="K200" s="5">
         <v>0.4</v>
       </c>
+      <c r="N200">
+        <v>2</v>
+      </c>
+      <c r="O200">
+        <v>1</v>
+      </c>
       <c r="P200" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.25">
@@ -7475,7 +7835,7 @@
         <v>1</v>
       </c>
       <c r="P201" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.25">
@@ -7513,7 +7873,7 @@
         <v>0.4</v>
       </c>
       <c r="P202" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.25">
@@ -7551,7 +7911,7 @@
         <v>0.4</v>
       </c>
       <c r="P203" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.25">
@@ -7589,7 +7949,7 @@
         <v>0.4</v>
       </c>
       <c r="P204" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.25">
@@ -7636,7 +7996,7 @@
         <v>1</v>
       </c>
       <c r="P205" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.25">
@@ -7674,7 +8034,7 @@
         <v>0.4</v>
       </c>
       <c r="P206" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="207" spans="1:16" x14ac:dyDescent="0.25">
@@ -7712,7 +8072,7 @@
         <v>0.4</v>
       </c>
       <c r="P207" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="208" spans="1:16" x14ac:dyDescent="0.25">
@@ -7750,7 +8110,7 @@
         <v>0.4</v>
       </c>
       <c r="P208" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="209" spans="1:16" x14ac:dyDescent="0.25">
@@ -7788,7 +8148,7 @@
         <v>0.4</v>
       </c>
       <c r="P209" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="210" spans="1:16" x14ac:dyDescent="0.25">
@@ -7829,7 +8189,7 @@
         <v>0.4</v>
       </c>
       <c r="P210" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="211" spans="1:16" x14ac:dyDescent="0.25">
@@ -7876,7 +8236,7 @@
         <v>1</v>
       </c>
       <c r="P211" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="212" spans="1:16" x14ac:dyDescent="0.25">
@@ -7914,7 +8274,7 @@
         <v>0.4</v>
       </c>
       <c r="P212" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="213" spans="1:16" x14ac:dyDescent="0.25">
@@ -7952,7 +8312,7 @@
         <v>0.4</v>
       </c>
       <c r="P213" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="214" spans="1:16" x14ac:dyDescent="0.25">
@@ -7996,7 +8356,7 @@
         <v>1</v>
       </c>
       <c r="P214" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="215" spans="1:16" x14ac:dyDescent="0.25">
@@ -8034,7 +8394,7 @@
         <v>0.4</v>
       </c>
       <c r="P215" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="216" spans="1:16" x14ac:dyDescent="0.25">
@@ -8063,16 +8423,22 @@
         <v>0</v>
       </c>
       <c r="I216" s="5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J216" s="5">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="K216" s="5">
-        <v>0.4</v>
+        <v>1.4</v>
+      </c>
+      <c r="N216">
+        <v>1</v>
+      </c>
+      <c r="O216">
+        <v>1</v>
       </c>
       <c r="P216" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="217" spans="1:16" x14ac:dyDescent="0.25">
@@ -8110,10 +8476,16 @@
         <v>1</v>
       </c>
       <c r="K217" s="5">
-        <v>0.4</v>
+        <v>1.4</v>
+      </c>
+      <c r="N217">
+        <v>1</v>
+      </c>
+      <c r="O217">
+        <v>1</v>
       </c>
       <c r="P217" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="218" spans="1:16" x14ac:dyDescent="0.25">
@@ -8151,7 +8523,7 @@
         <v>0.4</v>
       </c>
       <c r="P218" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="219" spans="1:16" x14ac:dyDescent="0.25">
@@ -8198,7 +8570,7 @@
         <v>1</v>
       </c>
       <c r="P219" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="220" spans="1:16" x14ac:dyDescent="0.25">
@@ -8236,7 +8608,7 @@
         <v>0.4</v>
       </c>
       <c r="P220" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="221" spans="1:16" x14ac:dyDescent="0.25">
@@ -8274,7 +8646,7 @@
         <v>0.4</v>
       </c>
       <c r="P221" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="222" spans="1:16" x14ac:dyDescent="0.25">
@@ -8318,7 +8690,7 @@
         <v>1</v>
       </c>
       <c r="P222" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="223" spans="1:16" x14ac:dyDescent="0.25">
@@ -8356,7 +8728,7 @@
         <v>0.4</v>
       </c>
       <c r="P223" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="224" spans="1:16" x14ac:dyDescent="0.25">
@@ -8394,7 +8766,7 @@
         <v>0.4</v>
       </c>
       <c r="P224" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="225" spans="1:16" x14ac:dyDescent="0.25">
@@ -8438,7 +8810,7 @@
         <v>1</v>
       </c>
       <c r="P225" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="226" spans="1:16" x14ac:dyDescent="0.25">
@@ -8476,7 +8848,7 @@
         <v>0.4</v>
       </c>
       <c r="P226" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="227" spans="1:16" x14ac:dyDescent="0.25">
@@ -8514,7 +8886,7 @@
         <v>0.4</v>
       </c>
       <c r="P227" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="228" spans="1:16" x14ac:dyDescent="0.25">
@@ -8552,7 +8924,7 @@
         <v>0.4</v>
       </c>
       <c r="P228" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="229" spans="1:16" x14ac:dyDescent="0.25">
@@ -8590,7 +8962,7 @@
         <v>0.4</v>
       </c>
       <c r="P229" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="230" spans="1:16" x14ac:dyDescent="0.25">
@@ -8628,7 +9000,7 @@
         <v>0.4</v>
       </c>
       <c r="P230" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="231" spans="1:16" x14ac:dyDescent="0.25">
@@ -8660,13 +9032,19 @@
         <v>0</v>
       </c>
       <c r="J231">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="K231">
-        <v>0.4</v>
+        <v>1.4</v>
+      </c>
+      <c r="N231">
+        <v>1</v>
+      </c>
+      <c r="O231">
+        <v>1</v>
       </c>
       <c r="P231" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="232" spans="1:16" x14ac:dyDescent="0.25">
@@ -8710,7 +9088,7 @@
         <v>1</v>
       </c>
       <c r="P232" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="233" spans="1:16" x14ac:dyDescent="0.25">
@@ -8742,13 +9120,19 @@
         <v>0</v>
       </c>
       <c r="J233">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="K233">
-        <v>0.4</v>
+        <v>1.4</v>
+      </c>
+      <c r="N233">
+        <v>1</v>
+      </c>
+      <c r="O233">
+        <v>1</v>
       </c>
       <c r="P233" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="234" spans="1:16" x14ac:dyDescent="0.25">
@@ -8792,7 +9176,7 @@
         <v>1</v>
       </c>
       <c r="P234" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="235" spans="1:16" x14ac:dyDescent="0.25">
@@ -8830,7 +9214,7 @@
         <v>0.4</v>
       </c>
       <c r="P235" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="236" spans="1:16" x14ac:dyDescent="0.25">
@@ -8868,7 +9252,7 @@
         <v>0.4</v>
       </c>
       <c r="P236" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="237" spans="1:16" x14ac:dyDescent="0.25">
@@ -8906,7 +9290,7 @@
         <v>0.4</v>
       </c>
       <c r="P237" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="238" spans="1:16" x14ac:dyDescent="0.25">
@@ -8944,7 +9328,7 @@
         <v>0.4</v>
       </c>
       <c r="P238" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="239" spans="1:16" x14ac:dyDescent="0.25">
@@ -8982,7 +9366,7 @@
         <v>0.4</v>
       </c>
       <c r="P239" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="240" spans="1:16" x14ac:dyDescent="0.25">
@@ -9026,7 +9410,7 @@
         <v>2</v>
       </c>
       <c r="P240" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="241" spans="1:16" x14ac:dyDescent="0.25">
@@ -9070,7 +9454,7 @@
         <v>2</v>
       </c>
       <c r="P241" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="242" spans="1:16" x14ac:dyDescent="0.25">
@@ -9114,7 +9498,7 @@
         <v>2</v>
       </c>
       <c r="P242" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="243" spans="1:16" x14ac:dyDescent="0.25">
@@ -9158,7 +9542,7 @@
         <v>2</v>
       </c>
       <c r="P243" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="244" spans="1:16" x14ac:dyDescent="0.25">
@@ -9202,7 +9586,7 @@
         <v>2</v>
       </c>
       <c r="P244" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="245" spans="1:16" x14ac:dyDescent="0.25">
@@ -9246,7 +9630,7 @@
         <v>2</v>
       </c>
       <c r="P245" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="246" spans="1:16" x14ac:dyDescent="0.25">
@@ -9290,7 +9674,7 @@
         <v>2</v>
       </c>
       <c r="P246" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="247" spans="1:16" x14ac:dyDescent="0.25">
@@ -9334,7 +9718,7 @@
         <v>2</v>
       </c>
       <c r="P247" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="248" spans="1:16" x14ac:dyDescent="0.25">
@@ -9378,7 +9762,7 @@
         <v>2</v>
       </c>
       <c r="P248" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="249" spans="1:16" x14ac:dyDescent="0.25">
@@ -9422,7 +9806,7 @@
         <v>2</v>
       </c>
       <c r="P249" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="250" spans="1:16" x14ac:dyDescent="0.25">
@@ -9466,7 +9850,7 @@
         <v>2</v>
       </c>
       <c r="P250" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="251" spans="1:16" x14ac:dyDescent="0.25">
@@ -9510,7 +9894,7 @@
         <v>2</v>
       </c>
       <c r="P251" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="252" spans="1:16" x14ac:dyDescent="0.25">
@@ -9554,7 +9938,7 @@
         <v>2</v>
       </c>
       <c r="P252" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="253" spans="1:16" x14ac:dyDescent="0.25">
@@ -9598,7 +9982,7 @@
         <v>2</v>
       </c>
       <c r="P253" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="254" spans="1:16" x14ac:dyDescent="0.25">
@@ -9642,7 +10026,7 @@
         <v>2</v>
       </c>
       <c r="P254" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="255" spans="1:16" x14ac:dyDescent="0.25">
@@ -9686,7 +10070,7 @@
         <v>2</v>
       </c>
       <c r="P255" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="256" spans="1:16" x14ac:dyDescent="0.25">
@@ -9730,7 +10114,7 @@
         <v>2</v>
       </c>
       <c r="P256" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="257" spans="1:16" x14ac:dyDescent="0.25">
@@ -9774,7 +10158,7 @@
         <v>2</v>
       </c>
       <c r="P257" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
     </row>
     <row r="258" spans="1:16" x14ac:dyDescent="0.25">
@@ -9818,7 +10202,7 @@
         <v>1</v>
       </c>
       <c r="P258" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="259" spans="1:16" x14ac:dyDescent="0.25">
@@ -9862,7 +10246,7 @@
         <v>1</v>
       </c>
       <c r="P259" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="260" spans="1:16" x14ac:dyDescent="0.25">
@@ -9888,7 +10272,7 @@
         <v>1.25</v>
       </c>
       <c r="H260">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I260">
         <v>0</v>
@@ -9899,8 +10283,14 @@
       <c r="K260">
         <v>1.5</v>
       </c>
-      <c r="P260" t="s">
-        <v>63</v>
+      <c r="N260">
+        <v>1</v>
+      </c>
+      <c r="O260">
+        <v>1</v>
+      </c>
+      <c r="P260" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="261" spans="1:16" x14ac:dyDescent="0.25">
@@ -9944,7 +10334,7 @@
         <v>1</v>
       </c>
       <c r="P261" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="262" spans="1:16" x14ac:dyDescent="0.25">
@@ -9988,7 +10378,7 @@
         <v>1</v>
       </c>
       <c r="P262" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="263" spans="1:16" x14ac:dyDescent="0.25">
@@ -10026,7 +10416,7 @@
         <v>1</v>
       </c>
       <c r="P263" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="264" spans="1:16" x14ac:dyDescent="0.25">
@@ -10064,7 +10454,7 @@
         <v>1</v>
       </c>
       <c r="P264" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="265" spans="1:16" x14ac:dyDescent="0.25">
@@ -10108,7 +10498,7 @@
         <v>1</v>
       </c>
       <c r="P265" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="266" spans="1:16" x14ac:dyDescent="0.25">
@@ -10152,7 +10542,7 @@
         <v>1</v>
       </c>
       <c r="P266" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="267" spans="1:16" x14ac:dyDescent="0.25">
@@ -10196,7 +10586,7 @@
         <v>1</v>
       </c>
       <c r="P267" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="268" spans="1:16" x14ac:dyDescent="0.25">
@@ -10240,7 +10630,7 @@
         <v>1</v>
       </c>
       <c r="P268" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="269" spans="1:16" x14ac:dyDescent="0.25">
@@ -10278,7 +10668,7 @@
         <v>1</v>
       </c>
       <c r="P269" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="270" spans="1:16" x14ac:dyDescent="0.25">
@@ -10316,7 +10706,7 @@
         <v>1</v>
       </c>
       <c r="P270" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="271" spans="1:16" x14ac:dyDescent="0.25">
@@ -10360,7 +10750,7 @@
         <v>1</v>
       </c>
       <c r="P271" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="272" spans="1:16" x14ac:dyDescent="0.25">
@@ -10404,7 +10794,7 @@
         <v>1</v>
       </c>
       <c r="P272" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="273" spans="1:16" x14ac:dyDescent="0.25">
@@ -10448,7 +10838,7 @@
         <v>5</v>
       </c>
       <c r="P273" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="274" spans="1:16" x14ac:dyDescent="0.25">
@@ -10492,7 +10882,7 @@
         <v>10</v>
       </c>
       <c r="P274" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="275" spans="1:16" x14ac:dyDescent="0.25">
@@ -10536,7 +10926,7 @@
         <v>10</v>
       </c>
       <c r="P275" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="276" spans="1:16" x14ac:dyDescent="0.25">
@@ -10580,7 +10970,7 @@
         <v>5</v>
       </c>
       <c r="P276" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="277" spans="1:16" x14ac:dyDescent="0.25">
@@ -10624,7 +11014,7 @@
         <v>1</v>
       </c>
       <c r="P277" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="278" spans="1:16" x14ac:dyDescent="0.25">
@@ -10668,7 +11058,7 @@
         <v>1</v>
       </c>
       <c r="P278" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="279" spans="1:16" x14ac:dyDescent="0.25">
@@ -10703,10 +11093,16 @@
         <v>1</v>
       </c>
       <c r="K279">
-        <v>1.2</v>
+        <v>1.4</v>
+      </c>
+      <c r="N279">
+        <v>1</v>
+      </c>
+      <c r="O279">
+        <v>1</v>
       </c>
       <c r="P279" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="280" spans="1:16" x14ac:dyDescent="0.25">
@@ -10750,7 +11146,7 @@
         <v>1</v>
       </c>
       <c r="P280" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="281" spans="1:16" x14ac:dyDescent="0.25">
@@ -10794,7 +11190,7 @@
         <v>1</v>
       </c>
       <c r="P281" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="282" spans="1:16" x14ac:dyDescent="0.25">
@@ -10831,8 +11227,14 @@
       <c r="K282">
         <v>1.4</v>
       </c>
+      <c r="N282">
+        <v>1</v>
+      </c>
+      <c r="O282">
+        <v>1</v>
+      </c>
       <c r="P282" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="283" spans="1:16" x14ac:dyDescent="0.25">
@@ -10882,7 +11284,7 @@
         <v>1</v>
       </c>
       <c r="P283" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="284" spans="1:16" x14ac:dyDescent="0.25">
@@ -10926,7 +11328,7 @@
         <v>1</v>
       </c>
       <c r="P284" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="285" spans="1:16" x14ac:dyDescent="0.25">
@@ -10970,7 +11372,7 @@
         <v>1</v>
       </c>
       <c r="P285" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="286" spans="1:16" x14ac:dyDescent="0.25">
@@ -11005,10 +11407,16 @@
         <v>1</v>
       </c>
       <c r="K286">
-        <v>1.2</v>
+        <v>1.4</v>
+      </c>
+      <c r="N286">
+        <v>1</v>
+      </c>
+      <c r="O286">
+        <v>1</v>
       </c>
       <c r="P286" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="287" spans="1:16" x14ac:dyDescent="0.25">
@@ -11052,7 +11460,7 @@
         <v>1</v>
       </c>
       <c r="P287" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="288" spans="1:16" x14ac:dyDescent="0.25">
@@ -11096,7 +11504,7 @@
         <v>1</v>
       </c>
       <c r="P288" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="289" spans="1:16" x14ac:dyDescent="0.25">
@@ -11125,16 +11533,22 @@
         <v>0</v>
       </c>
       <c r="I289">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="J289">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="K289">
         <v>1.4</v>
       </c>
+      <c r="N289">
+        <v>1</v>
+      </c>
+      <c r="O289">
+        <v>1</v>
+      </c>
       <c r="P289" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="290" spans="1:16" x14ac:dyDescent="0.25">
@@ -11178,7 +11592,7 @@
         <v>10</v>
       </c>
       <c r="P290" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="291" spans="1:16" x14ac:dyDescent="0.25">
@@ -11222,7 +11636,7 @@
         <v>1</v>
       </c>
       <c r="P291" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="292" spans="1:16" x14ac:dyDescent="0.25">
@@ -11266,7 +11680,7 @@
         <v>1</v>
       </c>
       <c r="P292" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="293" spans="1:16" x14ac:dyDescent="0.25">
@@ -11301,10 +11715,16 @@
         <v>1</v>
       </c>
       <c r="K293">
-        <v>1.2</v>
+        <v>1.4</v>
+      </c>
+      <c r="N293">
+        <v>1</v>
+      </c>
+      <c r="O293">
+        <v>1</v>
       </c>
       <c r="P293" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="294" spans="1:16" x14ac:dyDescent="0.25">
@@ -11348,7 +11768,7 @@
         <v>1</v>
       </c>
       <c r="P294" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="295" spans="1:16" x14ac:dyDescent="0.25">
@@ -11392,7 +11812,7 @@
         <v>1</v>
       </c>
       <c r="P295" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="296" spans="1:16" x14ac:dyDescent="0.25">
@@ -11421,16 +11841,22 @@
         <v>0</v>
       </c>
       <c r="I296">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="J296">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="K296">
         <v>1.4</v>
       </c>
+      <c r="N296">
+        <v>1</v>
+      </c>
+      <c r="O296">
+        <v>1</v>
+      </c>
       <c r="P296" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="297" spans="1:16" x14ac:dyDescent="0.25">
@@ -11474,7 +11900,7 @@
         <v>10</v>
       </c>
       <c r="P297" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="298" spans="1:16" x14ac:dyDescent="0.25">
@@ -11518,7 +11944,7 @@
         <v>1</v>
       </c>
       <c r="P298" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="299" spans="1:16" x14ac:dyDescent="0.25">
@@ -11562,7 +11988,7 @@
         <v>1</v>
       </c>
       <c r="P299" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="300" spans="1:16" x14ac:dyDescent="0.25">
@@ -11597,10 +12023,16 @@
         <v>1</v>
       </c>
       <c r="K300">
-        <v>1.2</v>
+        <v>1.4</v>
+      </c>
+      <c r="N300">
+        <v>1</v>
+      </c>
+      <c r="O300">
+        <v>1</v>
       </c>
       <c r="P300" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="301" spans="1:16" x14ac:dyDescent="0.25">
@@ -11644,7 +12076,7 @@
         <v>1</v>
       </c>
       <c r="P301" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="302" spans="1:16" x14ac:dyDescent="0.25">
@@ -11688,7 +12120,7 @@
         <v>1</v>
       </c>
       <c r="P302" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="303" spans="1:16" x14ac:dyDescent="0.25">
@@ -11717,16 +12149,22 @@
         <v>0</v>
       </c>
       <c r="I303">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="J303">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="K303">
         <v>1.4</v>
       </c>
+      <c r="N303">
+        <v>1</v>
+      </c>
+      <c r="O303">
+        <v>1</v>
+      </c>
       <c r="P303" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="304" spans="1:16" x14ac:dyDescent="0.25">
@@ -11770,7 +12208,7 @@
         <v>1</v>
       </c>
       <c r="P304" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="305" spans="1:16" x14ac:dyDescent="0.25">
@@ -11814,7 +12252,7 @@
         <v>1</v>
       </c>
       <c r="P305" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="306" spans="1:16" x14ac:dyDescent="0.25">
@@ -11849,10 +12287,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="K306">
-        <v>1.2</v>
+        <v>1.4</v>
+      </c>
+      <c r="N306">
+        <v>1</v>
+      </c>
+      <c r="O306">
+        <v>1</v>
       </c>
       <c r="P306" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="307" spans="1:16" x14ac:dyDescent="0.25">
@@ -11896,7 +12340,7 @@
         <v>1</v>
       </c>
       <c r="P307" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="308" spans="1:16" x14ac:dyDescent="0.25">
@@ -11940,7 +12384,7 @@
         <v>1</v>
       </c>
       <c r="P308" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="309" spans="1:16" x14ac:dyDescent="0.25">
@@ -11969,16 +12413,1650 @@
         <v>0</v>
       </c>
       <c r="I309">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="J309">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="K309">
         <v>1.4</v>
       </c>
+      <c r="N309">
+        <v>1</v>
+      </c>
+      <c r="O309">
+        <v>1</v>
+      </c>
       <c r="P309" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="310" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A310" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B310">
+        <v>44</v>
+      </c>
+      <c r="C310">
+        <v>2</v>
+      </c>
+      <c r="D310" t="s">
+        <v>5</v>
+      </c>
+      <c r="E310">
+        <v>0.01</v>
+      </c>
+      <c r="F310">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G310">
+        <v>12.5</v>
+      </c>
+      <c r="H310">
+        <v>0</v>
+      </c>
+      <c r="I310">
+        <v>-0.5</v>
+      </c>
+      <c r="J310">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K310">
+        <v>1.4</v>
+      </c>
+      <c r="N310">
+        <v>1</v>
+      </c>
+      <c r="O310">
+        <v>1</v>
+      </c>
+      <c r="P310" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="311" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A311" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B311">
+        <v>44</v>
+      </c>
+      <c r="C311">
+        <v>3</v>
+      </c>
+      <c r="D311" t="s">
+        <v>5</v>
+      </c>
+      <c r="E311">
+        <v>0.01</v>
+      </c>
+      <c r="F311">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G311">
+        <v>12.5</v>
+      </c>
+      <c r="H311">
+        <v>0</v>
+      </c>
+      <c r="I311">
+        <v>-0.5</v>
+      </c>
+      <c r="J311">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K311">
+        <v>1.4</v>
+      </c>
+      <c r="N311">
+        <v>1</v>
+      </c>
+      <c r="O311">
+        <v>1</v>
+      </c>
+      <c r="P311" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="312" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A312" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B312">
+        <v>44</v>
+      </c>
+      <c r="C312">
+        <v>4</v>
+      </c>
+      <c r="D312" t="s">
+        <v>5</v>
+      </c>
+      <c r="E312">
+        <v>0.01</v>
+      </c>
+      <c r="F312">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G312">
+        <v>12.5</v>
+      </c>
+      <c r="H312">
+        <v>0</v>
+      </c>
+      <c r="I312">
+        <v>-0.5</v>
+      </c>
+      <c r="J312">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K312">
+        <v>1.4</v>
+      </c>
+      <c r="N312">
+        <v>1</v>
+      </c>
+      <c r="O312">
+        <v>1</v>
+      </c>
+      <c r="P312" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="313" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A313" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B313">
+        <v>44</v>
+      </c>
+      <c r="C313">
+        <v>5</v>
+      </c>
+      <c r="D313" t="s">
+        <v>5</v>
+      </c>
+      <c r="E313">
+        <v>0.01</v>
+      </c>
+      <c r="F313">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G313">
+        <v>12.5</v>
+      </c>
+      <c r="H313">
+        <v>0</v>
+      </c>
+      <c r="I313">
+        <v>-0.5</v>
+      </c>
+      <c r="J313">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K313">
+        <v>1.4</v>
+      </c>
+      <c r="N313">
+        <v>1</v>
+      </c>
+      <c r="O313">
+        <v>1</v>
+      </c>
+      <c r="P313" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="314" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A314" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B314">
+        <v>44</v>
+      </c>
+      <c r="C314">
+        <v>6</v>
+      </c>
+      <c r="D314" t="s">
+        <v>5</v>
+      </c>
+      <c r="E314">
+        <v>0.01</v>
+      </c>
+      <c r="F314">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G314">
+        <v>12.5</v>
+      </c>
+      <c r="H314">
+        <v>0</v>
+      </c>
+      <c r="I314">
+        <v>-0.5</v>
+      </c>
+      <c r="J314">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K314">
+        <v>1.4</v>
+      </c>
+      <c r="N314">
+        <v>1</v>
+      </c>
+      <c r="O314">
+        <v>1</v>
+      </c>
+      <c r="P314" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="315" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A315" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B315">
+        <v>44</v>
+      </c>
+      <c r="C315">
+        <v>8</v>
+      </c>
+      <c r="D315" t="s">
+        <v>5</v>
+      </c>
+      <c r="E315">
+        <v>0.01</v>
+      </c>
+      <c r="F315">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G315">
+        <v>12.5</v>
+      </c>
+      <c r="H315">
+        <v>0</v>
+      </c>
+      <c r="I315">
+        <v>-0.5</v>
+      </c>
+      <c r="J315">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K315">
+        <v>1.4</v>
+      </c>
+      <c r="N315">
+        <v>1</v>
+      </c>
+      <c r="O315">
+        <v>1</v>
+      </c>
+      <c r="P315" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="316" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A316" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B316">
+        <v>44</v>
+      </c>
+      <c r="C316">
+        <v>9</v>
+      </c>
+      <c r="D316" t="s">
+        <v>5</v>
+      </c>
+      <c r="E316">
+        <v>0.01</v>
+      </c>
+      <c r="F316">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G316">
+        <v>12.5</v>
+      </c>
+      <c r="H316">
+        <v>0</v>
+      </c>
+      <c r="I316">
+        <v>-0.5</v>
+      </c>
+      <c r="J316">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K316">
+        <v>0.6</v>
+      </c>
+      <c r="N316">
+        <v>1</v>
+      </c>
+      <c r="O316">
+        <v>1</v>
+      </c>
+      <c r="P316" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="317" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A317" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B317">
+        <v>44</v>
+      </c>
+      <c r="C317">
+        <v>10</v>
+      </c>
+      <c r="D317" t="s">
+        <v>5</v>
+      </c>
+      <c r="E317">
+        <v>0.01</v>
+      </c>
+      <c r="F317">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G317">
+        <v>12.5</v>
+      </c>
+      <c r="H317">
+        <v>0</v>
+      </c>
+      <c r="I317">
+        <v>-0.5</v>
+      </c>
+      <c r="J317">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K317">
+        <v>1.4</v>
+      </c>
+      <c r="N317">
+        <v>1</v>
+      </c>
+      <c r="O317">
+        <v>1</v>
+      </c>
+      <c r="P317" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="318" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A318" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B318">
+        <v>44</v>
+      </c>
+      <c r="C318">
+        <v>11</v>
+      </c>
+      <c r="D318" t="s">
+        <v>5</v>
+      </c>
+      <c r="E318">
+        <v>0.01</v>
+      </c>
+      <c r="F318">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G318">
+        <v>12.5</v>
+      </c>
+      <c r="H318">
+        <v>0</v>
+      </c>
+      <c r="I318">
+        <v>-0.5</v>
+      </c>
+      <c r="J318">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K318">
+        <v>1.4</v>
+      </c>
+      <c r="N318">
+        <v>1</v>
+      </c>
+      <c r="O318">
+        <v>1</v>
+      </c>
+      <c r="P318" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="319" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A319" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B319">
+        <v>44</v>
+      </c>
+      <c r="C319">
+        <v>12</v>
+      </c>
+      <c r="D319" t="s">
+        <v>5</v>
+      </c>
+      <c r="E319">
+        <v>0.01</v>
+      </c>
+      <c r="F319">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G319">
+        <v>12.5</v>
+      </c>
+      <c r="H319">
+        <v>0</v>
+      </c>
+      <c r="I319">
+        <v>-0.5</v>
+      </c>
+      <c r="J319">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K319">
+        <v>1.4</v>
+      </c>
+      <c r="N319">
+        <v>1</v>
+      </c>
+      <c r="O319">
+        <v>1</v>
+      </c>
+      <c r="P319" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="320" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A320" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B320">
+        <v>44</v>
+      </c>
+      <c r="C320">
+        <v>13</v>
+      </c>
+      <c r="D320" t="s">
+        <v>5</v>
+      </c>
+      <c r="E320">
+        <v>0.01</v>
+      </c>
+      <c r="F320">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G320">
+        <v>12.5</v>
+      </c>
+      <c r="H320">
+        <v>0</v>
+      </c>
+      <c r="I320">
+        <v>-0.5</v>
+      </c>
+      <c r="J320">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K320">
+        <v>1.4</v>
+      </c>
+      <c r="N320">
+        <v>1</v>
+      </c>
+      <c r="O320">
+        <v>1</v>
+      </c>
+      <c r="P320" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="321" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A321" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B321">
+        <v>44</v>
+      </c>
+      <c r="C321">
+        <v>17</v>
+      </c>
+      <c r="D321" t="s">
+        <v>5</v>
+      </c>
+      <c r="E321">
+        <v>0.01</v>
+      </c>
+      <c r="F321">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G321">
+        <v>12.5</v>
+      </c>
+      <c r="H321">
+        <v>0</v>
+      </c>
+      <c r="I321">
+        <v>-0.5</v>
+      </c>
+      <c r="J321">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K321">
+        <v>1.4</v>
+      </c>
+      <c r="N321">
+        <v>1</v>
+      </c>
+      <c r="O321">
+        <v>1</v>
+      </c>
+      <c r="P321" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="322" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A322" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B322">
+        <v>44</v>
+      </c>
+      <c r="C322">
+        <v>18</v>
+      </c>
+      <c r="D322" t="s">
+        <v>5</v>
+      </c>
+      <c r="E322">
+        <v>0.01</v>
+      </c>
+      <c r="F322">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G322">
+        <v>12.5</v>
+      </c>
+      <c r="H322">
+        <v>0</v>
+      </c>
+      <c r="I322">
+        <v>-0.5</v>
+      </c>
+      <c r="J322">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K322">
+        <v>1.4</v>
+      </c>
+      <c r="N322">
+        <v>1</v>
+      </c>
+      <c r="O322">
+        <v>1</v>
+      </c>
+      <c r="P322" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="323" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A323" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B323">
+        <v>44</v>
+      </c>
+      <c r="C323">
+        <v>19</v>
+      </c>
+      <c r="D323" t="s">
+        <v>5</v>
+      </c>
+      <c r="E323">
+        <v>0.02</v>
+      </c>
+      <c r="F323">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G323">
+        <v>6.25</v>
+      </c>
+      <c r="H323">
+        <v>0</v>
+      </c>
+      <c r="I323">
+        <v>-1.5</v>
+      </c>
+      <c r="J323">
+        <v>1.2</v>
+      </c>
+      <c r="K323">
+        <v>1.2</v>
+      </c>
+      <c r="N323">
+        <v>1</v>
+      </c>
+      <c r="O323">
+        <v>1</v>
+      </c>
+      <c r="P323" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="324" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A324" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B324">
+        <v>44</v>
+      </c>
+      <c r="C324">
+        <v>20</v>
+      </c>
+      <c r="D324" t="s">
+        <v>5</v>
+      </c>
+      <c r="E324">
+        <v>0.02</v>
+      </c>
+      <c r="F324">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G324">
+        <v>6.25</v>
+      </c>
+      <c r="H324">
+        <v>0</v>
+      </c>
+      <c r="I324">
+        <v>-1.5</v>
+      </c>
+      <c r="J324">
+        <v>1.2</v>
+      </c>
+      <c r="K324">
+        <v>1.2</v>
+      </c>
+      <c r="N324">
+        <v>1</v>
+      </c>
+      <c r="O324">
+        <v>1</v>
+      </c>
+      <c r="P324" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="325" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A325" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B325">
+        <v>44</v>
+      </c>
+      <c r="C325">
+        <v>21</v>
+      </c>
+      <c r="D325" t="s">
+        <v>5</v>
+      </c>
+      <c r="E325">
+        <v>0.02</v>
+      </c>
+      <c r="F325">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G325">
+        <v>6.25</v>
+      </c>
+      <c r="H325">
+        <v>0</v>
+      </c>
+      <c r="I325">
+        <v>-1.5</v>
+      </c>
+      <c r="J325">
+        <v>1.2</v>
+      </c>
+      <c r="K325">
+        <v>1.2</v>
+      </c>
+      <c r="N325">
+        <v>1</v>
+      </c>
+      <c r="O325">
+        <v>1</v>
+      </c>
+      <c r="P325" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="326" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A326" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B326">
+        <v>44</v>
+      </c>
+      <c r="C326">
+        <v>22</v>
+      </c>
+      <c r="D326" t="s">
+        <v>5</v>
+      </c>
+      <c r="E326">
+        <v>0.02</v>
+      </c>
+      <c r="F326">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G326">
+        <v>6.25</v>
+      </c>
+      <c r="H326">
+        <v>0</v>
+      </c>
+      <c r="I326">
+        <v>-1.5</v>
+      </c>
+      <c r="J326">
+        <v>1.2</v>
+      </c>
+      <c r="K326">
+        <v>1.2</v>
+      </c>
+      <c r="N326">
+        <v>1</v>
+      </c>
+      <c r="O326">
+        <v>1</v>
+      </c>
+      <c r="P326" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="327" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A327" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B327">
+        <v>45</v>
+      </c>
+      <c r="C327">
+        <v>25</v>
+      </c>
+      <c r="D327" t="s">
+        <v>5</v>
+      </c>
+      <c r="E327">
+        <v>0.01</v>
+      </c>
+      <c r="F327">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G327">
+        <v>12.5</v>
+      </c>
+      <c r="H327">
+        <v>0</v>
+      </c>
+      <c r="I327">
+        <v>-0.5</v>
+      </c>
+      <c r="J327">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K327">
+        <v>1.4</v>
+      </c>
+      <c r="N327">
+        <v>1</v>
+      </c>
+      <c r="O327">
+        <v>1</v>
+      </c>
+      <c r="P327" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="328" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A328" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B328">
+        <v>45</v>
+      </c>
+      <c r="C328">
+        <v>26</v>
+      </c>
+      <c r="D328" t="s">
+        <v>5</v>
+      </c>
+      <c r="E328">
+        <v>0.01</v>
+      </c>
+      <c r="F328">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G328">
+        <v>12.5</v>
+      </c>
+      <c r="H328">
+        <v>0</v>
+      </c>
+      <c r="I328">
+        <v>-0.5</v>
+      </c>
+      <c r="J328">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K328">
+        <v>1.4</v>
+      </c>
+      <c r="N328">
+        <v>1</v>
+      </c>
+      <c r="O328">
+        <v>1</v>
+      </c>
+      <c r="P328" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="329" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A329" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B329">
+        <v>45</v>
+      </c>
+      <c r="C329">
+        <v>27</v>
+      </c>
+      <c r="D329" t="s">
+        <v>5</v>
+      </c>
+      <c r="E329">
+        <v>0.01</v>
+      </c>
+      <c r="F329">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G329">
+        <v>12.5</v>
+      </c>
+      <c r="H329">
+        <v>0</v>
+      </c>
+      <c r="I329">
+        <v>-0.5</v>
+      </c>
+      <c r="J329">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K329">
+        <v>1.4</v>
+      </c>
+      <c r="N329">
+        <v>1</v>
+      </c>
+      <c r="O329">
+        <v>1</v>
+      </c>
+      <c r="P329" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="330" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A330" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B330">
+        <v>45</v>
+      </c>
+      <c r="C330">
+        <v>28</v>
+      </c>
+      <c r="D330" t="s">
+        <v>5</v>
+      </c>
+      <c r="E330">
+        <v>0.01</v>
+      </c>
+      <c r="F330">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G330">
+        <v>12.5</v>
+      </c>
+      <c r="H330">
+        <v>0</v>
+      </c>
+      <c r="I330">
+        <v>-0.5</v>
+      </c>
+      <c r="J330">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K330">
+        <v>1.4</v>
+      </c>
+      <c r="N330">
+        <v>1</v>
+      </c>
+      <c r="O330">
+        <v>1</v>
+      </c>
+      <c r="P330" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="331" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A331" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B331">
+        <v>45</v>
+      </c>
+      <c r="C331">
+        <v>29</v>
+      </c>
+      <c r="D331" t="s">
+        <v>5</v>
+      </c>
+      <c r="E331">
+        <v>0.01</v>
+      </c>
+      <c r="F331">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G331">
+        <v>12.5</v>
+      </c>
+      <c r="H331">
+        <v>0</v>
+      </c>
+      <c r="I331">
+        <v>-0.5</v>
+      </c>
+      <c r="J331">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K331">
+        <v>1.4</v>
+      </c>
+      <c r="N331">
+        <v>1</v>
+      </c>
+      <c r="O331">
+        <v>1</v>
+      </c>
+      <c r="P331" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="332" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A332" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B332">
+        <v>45</v>
+      </c>
+      <c r="C332">
+        <v>30</v>
+      </c>
+      <c r="D332" t="s">
+        <v>5</v>
+      </c>
+      <c r="E332">
+        <v>0.01</v>
+      </c>
+      <c r="F332">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G332">
+        <v>12.5</v>
+      </c>
+      <c r="H332">
+        <v>0</v>
+      </c>
+      <c r="I332">
+        <v>-0.5</v>
+      </c>
+      <c r="J332">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K332">
+        <v>1.4</v>
+      </c>
+      <c r="N332">
+        <v>1</v>
+      </c>
+      <c r="O332">
+        <v>1</v>
+      </c>
+      <c r="P332" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="333" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A333" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B333">
+        <v>45</v>
+      </c>
+      <c r="C333">
+        <v>31</v>
+      </c>
+      <c r="D333" t="s">
+        <v>5</v>
+      </c>
+      <c r="E333">
+        <v>0.01</v>
+      </c>
+      <c r="F333">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G333">
+        <v>12.5</v>
+      </c>
+      <c r="H333">
+        <v>0</v>
+      </c>
+      <c r="I333">
+        <v>-0.5</v>
+      </c>
+      <c r="J333">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K333">
+        <v>1.4</v>
+      </c>
+      <c r="N333">
+        <v>1</v>
+      </c>
+      <c r="O333">
+        <v>1</v>
+      </c>
+      <c r="P333" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="334" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A334" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B334">
+        <v>45</v>
+      </c>
+      <c r="C334">
+        <v>32</v>
+      </c>
+      <c r="D334" t="s">
+        <v>5</v>
+      </c>
+      <c r="E334">
+        <v>0.01</v>
+      </c>
+      <c r="F334">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G334">
+        <v>12.5</v>
+      </c>
+      <c r="H334">
+        <v>0</v>
+      </c>
+      <c r="I334">
+        <v>-0.5</v>
+      </c>
+      <c r="J334">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K334">
+        <v>1.4</v>
+      </c>
+      <c r="N334">
+        <v>1</v>
+      </c>
+      <c r="O334">
+        <v>1</v>
+      </c>
+      <c r="P334" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="335" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A335" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B335">
+        <v>45</v>
+      </c>
+      <c r="C335">
+        <v>33</v>
+      </c>
+      <c r="D335" t="s">
+        <v>5</v>
+      </c>
+      <c r="E335">
+        <v>0.01</v>
+      </c>
+      <c r="F335">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G335">
+        <v>12.5</v>
+      </c>
+      <c r="H335">
+        <v>0</v>
+      </c>
+      <c r="I335">
+        <v>-0.5</v>
+      </c>
+      <c r="J335">
+        <v>1.3</v>
+      </c>
+      <c r="K335">
+        <v>1.4</v>
+      </c>
+      <c r="N335">
+        <v>1</v>
+      </c>
+      <c r="O335">
+        <v>1</v>
+      </c>
+      <c r="P335" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="336" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A336" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B336">
+        <v>45</v>
+      </c>
+      <c r="C336">
+        <v>34</v>
+      </c>
+      <c r="D336" t="s">
+        <v>5</v>
+      </c>
+      <c r="E336">
+        <v>0.01</v>
+      </c>
+      <c r="F336">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G336">
+        <v>12.5</v>
+      </c>
+      <c r="H336">
+        <v>0</v>
+      </c>
+      <c r="I336">
+        <v>-0.5</v>
+      </c>
+      <c r="J336">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K336">
+        <v>1.4</v>
+      </c>
+      <c r="N336">
+        <v>1</v>
+      </c>
+      <c r="O336">
+        <v>1</v>
+      </c>
+      <c r="P336" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="337" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A337" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B337">
+        <v>45</v>
+      </c>
+      <c r="C337">
+        <v>35</v>
+      </c>
+      <c r="D337" t="s">
+        <v>5</v>
+      </c>
+      <c r="E337">
+        <v>0.01</v>
+      </c>
+      <c r="F337">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G337">
+        <v>12.5</v>
+      </c>
+      <c r="H337">
+        <v>0</v>
+      </c>
+      <c r="I337">
+        <v>-0.5</v>
+      </c>
+      <c r="J337">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K337">
+        <v>1.4</v>
+      </c>
+      <c r="N337">
+        <v>1</v>
+      </c>
+      <c r="O337">
+        <v>1</v>
+      </c>
+      <c r="P337" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="338" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A338" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B338">
+        <v>45</v>
+      </c>
+      <c r="C338">
+        <v>36</v>
+      </c>
+      <c r="D338" t="s">
+        <v>5</v>
+      </c>
+      <c r="E338">
+        <v>0.01</v>
+      </c>
+      <c r="F338">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G338">
+        <v>12.5</v>
+      </c>
+      <c r="H338">
+        <v>0</v>
+      </c>
+      <c r="I338">
+        <v>-0.5</v>
+      </c>
+      <c r="J338">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K338">
+        <v>1.4</v>
+      </c>
+      <c r="N338">
+        <v>1</v>
+      </c>
+      <c r="O338">
+        <v>1</v>
+      </c>
+      <c r="P338" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="339" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A339" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B339">
+        <v>45</v>
+      </c>
+      <c r="C339">
+        <v>37</v>
+      </c>
+      <c r="D339" t="s">
+        <v>5</v>
+      </c>
+      <c r="E339">
+        <v>0.01</v>
+      </c>
+      <c r="F339">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G339">
+        <v>12.5</v>
+      </c>
+      <c r="H339">
+        <v>0</v>
+      </c>
+      <c r="I339">
+        <v>-0.5</v>
+      </c>
+      <c r="J339">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K339">
+        <v>1.4</v>
+      </c>
+      <c r="N339">
+        <v>1</v>
+      </c>
+      <c r="O339">
+        <v>1</v>
+      </c>
+      <c r="P339" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="340" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A340" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B340">
+        <v>45</v>
+      </c>
+      <c r="C340">
+        <v>38</v>
+      </c>
+      <c r="D340" t="s">
+        <v>5</v>
+      </c>
+      <c r="E340">
+        <v>0.01</v>
+      </c>
+      <c r="F340">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G340">
+        <v>12.5</v>
+      </c>
+      <c r="H340">
+        <v>0</v>
+      </c>
+      <c r="I340">
+        <v>-0.5</v>
+      </c>
+      <c r="J340">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K340">
+        <v>1.4</v>
+      </c>
+      <c r="N340">
+        <v>1</v>
+      </c>
+      <c r="O340">
+        <v>1</v>
+      </c>
+      <c r="P340" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="341" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A341" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B341">
+        <v>45</v>
+      </c>
+      <c r="C341">
+        <v>39</v>
+      </c>
+      <c r="D341" t="s">
+        <v>5</v>
+      </c>
+      <c r="E341">
+        <v>0.01</v>
+      </c>
+      <c r="F341">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G341">
+        <v>12.5</v>
+      </c>
+      <c r="H341">
+        <v>0</v>
+      </c>
+      <c r="I341">
+        <v>-0.5</v>
+      </c>
+      <c r="J341">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K341">
+        <v>1.4</v>
+      </c>
+      <c r="N341">
+        <v>1</v>
+      </c>
+      <c r="O341">
+        <v>1</v>
+      </c>
+      <c r="P341" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="342" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A342" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B342">
+        <v>45</v>
+      </c>
+      <c r="C342">
+        <v>40</v>
+      </c>
+      <c r="D342" t="s">
+        <v>5</v>
+      </c>
+      <c r="E342">
+        <v>0.02</v>
+      </c>
+      <c r="F342">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G342">
+        <v>6.25</v>
+      </c>
+      <c r="H342">
+        <v>0</v>
+      </c>
+      <c r="I342">
+        <v>-1.5</v>
+      </c>
+      <c r="J342">
+        <v>1.2</v>
+      </c>
+      <c r="K342">
+        <v>1.2</v>
+      </c>
+      <c r="N342">
+        <v>1</v>
+      </c>
+      <c r="O342">
+        <v>1</v>
+      </c>
+      <c r="P342" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="343" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A343" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B343">
+        <v>45</v>
+      </c>
+      <c r="C343">
+        <v>41</v>
+      </c>
+      <c r="D343" t="s">
+        <v>5</v>
+      </c>
+      <c r="E343">
+        <v>0.02</v>
+      </c>
+      <c r="F343">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G343">
+        <v>6.25</v>
+      </c>
+      <c r="H343">
+        <v>0</v>
+      </c>
+      <c r="I343">
+        <v>-1.5</v>
+      </c>
+      <c r="J343">
+        <v>1.2</v>
+      </c>
+      <c r="K343">
+        <v>1.2</v>
+      </c>
+      <c r="N343">
+        <v>1</v>
+      </c>
+      <c r="O343">
+        <v>1</v>
+      </c>
+      <c r="P343" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="344" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A344" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B344">
+        <v>45</v>
+      </c>
+      <c r="C344">
+        <v>42</v>
+      </c>
+      <c r="D344" t="s">
+        <v>5</v>
+      </c>
+      <c r="E344">
+        <v>0.02</v>
+      </c>
+      <c r="F344">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G344">
+        <v>6.25</v>
+      </c>
+      <c r="H344">
+        <v>0</v>
+      </c>
+      <c r="I344">
+        <v>-1.5</v>
+      </c>
+      <c r="J344">
+        <v>1.2</v>
+      </c>
+      <c r="K344">
+        <v>1.2</v>
+      </c>
+      <c r="N344">
+        <v>1</v>
+      </c>
+      <c r="O344">
+        <v>1</v>
+      </c>
+      <c r="P344" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="345" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A345" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B345">
+        <v>45</v>
+      </c>
+      <c r="C345">
+        <v>43</v>
+      </c>
+      <c r="D345" t="s">
+        <v>5</v>
+      </c>
+      <c r="E345">
+        <v>0.02</v>
+      </c>
+      <c r="F345">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G345">
+        <v>6.25</v>
+      </c>
+      <c r="H345">
+        <v>0</v>
+      </c>
+      <c r="I345">
+        <v>-1.5</v>
+      </c>
+      <c r="J345">
+        <v>1.2</v>
+      </c>
+      <c r="K345">
+        <v>1.2</v>
+      </c>
+      <c r="N345">
+        <v>1</v>
+      </c>
+      <c r="O345">
+        <v>1</v>
+      </c>
+      <c r="P345" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="346" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A346" s="1">
+        <v>44862</v>
+      </c>
+      <c r="B346">
+        <v>44</v>
+      </c>
+      <c r="C346">
+        <v>47</v>
+      </c>
+      <c r="D346" t="s">
+        <v>5</v>
+      </c>
+      <c r="E346">
+        <v>0.01</v>
+      </c>
+      <c r="F346">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G346">
+        <v>12.5</v>
+      </c>
+      <c r="H346">
+        <v>1</v>
+      </c>
+      <c r="I346">
+        <v>-0.5</v>
+      </c>
+      <c r="J346">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K346">
+        <v>1</v>
+      </c>
+      <c r="N346">
+        <v>1</v>
+      </c>
+      <c r="O346">
+        <v>1</v>
+      </c>
+      <c r="P346" s="7" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>